<commit_message>
feat(annex-k3): tune tmc driver parameters
</commit_message>
<xml_diff>
--- a/doc/annex-k3/driver_tuning/Annex-K3-E_LDO-36STH17-1004AH(G8T)_TMC2209_Calculations.xlsx
+++ b/doc/annex-k3/driver_tuning/Annex-K3-E_LDO-36STH17-1004AH(G8T)_TMC2209_Calculations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Jedermann\TMCTechAccessPack\Chips\TMC2209\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/niels/Projects/_3D Printing/klipper-configuration/doc/annex-k3/driver_tuning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0BD36AF-B6A7-41B4-BA24-498A2244D5EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91FF85C5-0CB4-C346-AF99-921275EA1A10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2976" yWindow="984" windowWidth="23040" windowHeight="12660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2980" yWindow="980" windowWidth="23040" windowHeight="12660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Velocity Calculation" sheetId="1" r:id="rId1"/>
@@ -1242,7 +1242,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -1258,18 +1258,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1283,34 +1279,24 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1318,13 +1304,12 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1339,15 +1324,15 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="48" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="14" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="14" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="14" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="14" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="4" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1359,9 +1344,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="10" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -1378,14 +1361,11 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -1426,7 +1406,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1748,25 +1728,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.77734375" customWidth="1"/>
-    <col min="3" max="3" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.88671875" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" customWidth="1"/>
+    <col min="3" max="3" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
     <col min="6" max="6" width="11.6640625" customWidth="1"/>
     <col min="7" max="7" width="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>177</v>
       </c>
@@ -1778,7 +1758,7 @@
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
     </row>
-    <row r="2" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -1788,45 +1768,45 @@
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
     </row>
-    <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="45" t="s">
         <v>109</v>
       </c>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="59"/>
-      <c r="H3" s="59"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-    </row>
-    <row r="4" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+    </row>
+    <row r="4" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="10"/>
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="47" t="s">
         <v>93</v>
       </c>
-      <c r="C4" s="61"/>
-      <c r="D4" s="61"/>
-      <c r="E4" s="61"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="61"/>
-      <c r="H4" s="61"/>
-      <c r="I4" s="62"/>
-      <c r="J4" s="62"/>
-      <c r="K4" s="62"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="49"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B7" s="64">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B7" s="51">
         <v>60</v>
       </c>
       <c r="C7" t="s">
@@ -1855,7 +1835,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B8" s="9">
         <v>256</v>
       </c>
@@ -1878,31 +1858,30 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B9" s="87">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B9" s="74">
         <v>1.8</v>
       </c>
-      <c r="C9" s="34" t="s">
+      <c r="C9" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="34" t="s">
+      <c r="D9" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="34" t="s">
+      <c r="F9" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="35" t="s">
+      <c r="G9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="87">
+      <c r="H9" s="74">
         <v>12000000</v>
       </c>
-      <c r="I9" s="34"/>
-      <c r="J9" s="34" t="s">
+      <c r="J9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B10">
         <f>360/B9</f>
         <v>200</v>
@@ -1914,7 +1893,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B11">
         <f>B10*B8</f>
         <v>51200</v>
@@ -1926,26 +1905,26 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B12" s="87">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B12" s="74">
         <v>1</v>
       </c>
-      <c r="C12" s="35" t="s">
+      <c r="C12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="34" t="s">
+      <c r="D12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>193</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B15" s="86">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B15" s="73">
         <f>B25</f>
         <v>71582.78826666667</v>
       </c>
@@ -1959,7 +1938,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B16" s="3">
         <f>B15/$J$7/$B$11</f>
         <v>1</v>
@@ -1971,7 +1950,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B17" s="3">
         <f>B16*360</f>
         <v>360</v>
@@ -1983,7 +1962,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B18" s="3">
         <f>B17/$B$12</f>
         <v>360</v>
@@ -1995,7 +1974,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B19" s="3">
         <f>B15*H9/2^24</f>
         <v>51200</v>
@@ -2007,7 +1986,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B20" s="8">
         <f>B18/360</f>
         <v>1</v>
@@ -2019,20 +1998,20 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B21" s="8"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>192</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B23" s="85">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B23" s="72">
         <f>B7/60</f>
         <v>1</v>
       </c>
@@ -2046,7 +2025,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B24" s="3">
         <f>B23*360</f>
         <v>360</v>
@@ -2058,7 +2037,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B25" s="7">
         <f>B23*$B$11*$J$7</f>
         <v>71582.78826666667</v>
@@ -2070,20 +2049,20 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B26" s="7"/>
       <c r="C26" s="4"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>194</v>
       </c>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
-      <c r="B28" s="85">
+      <c r="B28" s="72">
         <f>B23</f>
         <v>1</v>
       </c>
@@ -2094,7 +2073,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B29" s="3">
         <f>B28*360</f>
         <v>360</v>
@@ -2106,7 +2085,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B30" s="3">
         <f>B28*B12</f>
         <v>1</v>
@@ -2118,7 +2097,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B31" s="3">
         <f>B30*360</f>
         <v>360</v>
@@ -2130,7 +2109,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B32" s="7">
         <f>B30*$B$11*$J$7</f>
         <v>71582.78826666667</v>
@@ -2142,15 +2121,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>195</v>
       </c>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B35" s="86">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B35" s="73">
         <f>B15</f>
         <v>71582.78826666667</v>
       </c>
@@ -2161,7 +2140,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B36" s="7">
         <f>MIN((2^20-1),2^24/B35*B8/256)</f>
         <v>234.375</v>
@@ -2183,294 +2162,294 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="22.88671875" style="18" customWidth="1"/>
-    <col min="4" max="4" width="5.5546875" customWidth="1"/>
-    <col min="5" max="5" width="14.44140625" customWidth="1"/>
-    <col min="8" max="8" width="12.77734375" customWidth="1"/>
-    <col min="258" max="258" width="22.88671875" customWidth="1"/>
-    <col min="260" max="260" width="5.5546875" customWidth="1"/>
-    <col min="261" max="261" width="14.44140625" customWidth="1"/>
-    <col min="514" max="514" width="22.88671875" customWidth="1"/>
-    <col min="516" max="516" width="5.5546875" customWidth="1"/>
-    <col min="517" max="517" width="14.44140625" customWidth="1"/>
-    <col min="770" max="770" width="22.88671875" customWidth="1"/>
-    <col min="772" max="772" width="5.5546875" customWidth="1"/>
-    <col min="773" max="773" width="14.44140625" customWidth="1"/>
-    <col min="1026" max="1026" width="22.88671875" customWidth="1"/>
-    <col min="1028" max="1028" width="5.5546875" customWidth="1"/>
-    <col min="1029" max="1029" width="14.44140625" customWidth="1"/>
-    <col min="1282" max="1282" width="22.88671875" customWidth="1"/>
-    <col min="1284" max="1284" width="5.5546875" customWidth="1"/>
-    <col min="1285" max="1285" width="14.44140625" customWidth="1"/>
-    <col min="1538" max="1538" width="22.88671875" customWidth="1"/>
-    <col min="1540" max="1540" width="5.5546875" customWidth="1"/>
-    <col min="1541" max="1541" width="14.44140625" customWidth="1"/>
-    <col min="1794" max="1794" width="22.88671875" customWidth="1"/>
-    <col min="1796" max="1796" width="5.5546875" customWidth="1"/>
-    <col min="1797" max="1797" width="14.44140625" customWidth="1"/>
-    <col min="2050" max="2050" width="22.88671875" customWidth="1"/>
-    <col min="2052" max="2052" width="5.5546875" customWidth="1"/>
-    <col min="2053" max="2053" width="14.44140625" customWidth="1"/>
-    <col min="2306" max="2306" width="22.88671875" customWidth="1"/>
-    <col min="2308" max="2308" width="5.5546875" customWidth="1"/>
-    <col min="2309" max="2309" width="14.44140625" customWidth="1"/>
-    <col min="2562" max="2562" width="22.88671875" customWidth="1"/>
-    <col min="2564" max="2564" width="5.5546875" customWidth="1"/>
-    <col min="2565" max="2565" width="14.44140625" customWidth="1"/>
-    <col min="2818" max="2818" width="22.88671875" customWidth="1"/>
-    <col min="2820" max="2820" width="5.5546875" customWidth="1"/>
-    <col min="2821" max="2821" width="14.44140625" customWidth="1"/>
-    <col min="3074" max="3074" width="22.88671875" customWidth="1"/>
-    <col min="3076" max="3076" width="5.5546875" customWidth="1"/>
-    <col min="3077" max="3077" width="14.44140625" customWidth="1"/>
-    <col min="3330" max="3330" width="22.88671875" customWidth="1"/>
-    <col min="3332" max="3332" width="5.5546875" customWidth="1"/>
-    <col min="3333" max="3333" width="14.44140625" customWidth="1"/>
-    <col min="3586" max="3586" width="22.88671875" customWidth="1"/>
-    <col min="3588" max="3588" width="5.5546875" customWidth="1"/>
-    <col min="3589" max="3589" width="14.44140625" customWidth="1"/>
-    <col min="3842" max="3842" width="22.88671875" customWidth="1"/>
-    <col min="3844" max="3844" width="5.5546875" customWidth="1"/>
-    <col min="3845" max="3845" width="14.44140625" customWidth="1"/>
-    <col min="4098" max="4098" width="22.88671875" customWidth="1"/>
-    <col min="4100" max="4100" width="5.5546875" customWidth="1"/>
-    <col min="4101" max="4101" width="14.44140625" customWidth="1"/>
-    <col min="4354" max="4354" width="22.88671875" customWidth="1"/>
-    <col min="4356" max="4356" width="5.5546875" customWidth="1"/>
-    <col min="4357" max="4357" width="14.44140625" customWidth="1"/>
-    <col min="4610" max="4610" width="22.88671875" customWidth="1"/>
-    <col min="4612" max="4612" width="5.5546875" customWidth="1"/>
-    <col min="4613" max="4613" width="14.44140625" customWidth="1"/>
-    <col min="4866" max="4866" width="22.88671875" customWidth="1"/>
-    <col min="4868" max="4868" width="5.5546875" customWidth="1"/>
-    <col min="4869" max="4869" width="14.44140625" customWidth="1"/>
-    <col min="5122" max="5122" width="22.88671875" customWidth="1"/>
-    <col min="5124" max="5124" width="5.5546875" customWidth="1"/>
-    <col min="5125" max="5125" width="14.44140625" customWidth="1"/>
-    <col min="5378" max="5378" width="22.88671875" customWidth="1"/>
-    <col min="5380" max="5380" width="5.5546875" customWidth="1"/>
-    <col min="5381" max="5381" width="14.44140625" customWidth="1"/>
-    <col min="5634" max="5634" width="22.88671875" customWidth="1"/>
-    <col min="5636" max="5636" width="5.5546875" customWidth="1"/>
-    <col min="5637" max="5637" width="14.44140625" customWidth="1"/>
-    <col min="5890" max="5890" width="22.88671875" customWidth="1"/>
-    <col min="5892" max="5892" width="5.5546875" customWidth="1"/>
-    <col min="5893" max="5893" width="14.44140625" customWidth="1"/>
-    <col min="6146" max="6146" width="22.88671875" customWidth="1"/>
-    <col min="6148" max="6148" width="5.5546875" customWidth="1"/>
-    <col min="6149" max="6149" width="14.44140625" customWidth="1"/>
-    <col min="6402" max="6402" width="22.88671875" customWidth="1"/>
-    <col min="6404" max="6404" width="5.5546875" customWidth="1"/>
-    <col min="6405" max="6405" width="14.44140625" customWidth="1"/>
-    <col min="6658" max="6658" width="22.88671875" customWidth="1"/>
-    <col min="6660" max="6660" width="5.5546875" customWidth="1"/>
-    <col min="6661" max="6661" width="14.44140625" customWidth="1"/>
-    <col min="6914" max="6914" width="22.88671875" customWidth="1"/>
-    <col min="6916" max="6916" width="5.5546875" customWidth="1"/>
-    <col min="6917" max="6917" width="14.44140625" customWidth="1"/>
-    <col min="7170" max="7170" width="22.88671875" customWidth="1"/>
-    <col min="7172" max="7172" width="5.5546875" customWidth="1"/>
-    <col min="7173" max="7173" width="14.44140625" customWidth="1"/>
-    <col min="7426" max="7426" width="22.88671875" customWidth="1"/>
-    <col min="7428" max="7428" width="5.5546875" customWidth="1"/>
-    <col min="7429" max="7429" width="14.44140625" customWidth="1"/>
-    <col min="7682" max="7682" width="22.88671875" customWidth="1"/>
-    <col min="7684" max="7684" width="5.5546875" customWidth="1"/>
-    <col min="7685" max="7685" width="14.44140625" customWidth="1"/>
-    <col min="7938" max="7938" width="22.88671875" customWidth="1"/>
-    <col min="7940" max="7940" width="5.5546875" customWidth="1"/>
-    <col min="7941" max="7941" width="14.44140625" customWidth="1"/>
-    <col min="8194" max="8194" width="22.88671875" customWidth="1"/>
-    <col min="8196" max="8196" width="5.5546875" customWidth="1"/>
-    <col min="8197" max="8197" width="14.44140625" customWidth="1"/>
-    <col min="8450" max="8450" width="22.88671875" customWidth="1"/>
-    <col min="8452" max="8452" width="5.5546875" customWidth="1"/>
-    <col min="8453" max="8453" width="14.44140625" customWidth="1"/>
-    <col min="8706" max="8706" width="22.88671875" customWidth="1"/>
-    <col min="8708" max="8708" width="5.5546875" customWidth="1"/>
-    <col min="8709" max="8709" width="14.44140625" customWidth="1"/>
-    <col min="8962" max="8962" width="22.88671875" customWidth="1"/>
-    <col min="8964" max="8964" width="5.5546875" customWidth="1"/>
-    <col min="8965" max="8965" width="14.44140625" customWidth="1"/>
-    <col min="9218" max="9218" width="22.88671875" customWidth="1"/>
-    <col min="9220" max="9220" width="5.5546875" customWidth="1"/>
-    <col min="9221" max="9221" width="14.44140625" customWidth="1"/>
-    <col min="9474" max="9474" width="22.88671875" customWidth="1"/>
-    <col min="9476" max="9476" width="5.5546875" customWidth="1"/>
-    <col min="9477" max="9477" width="14.44140625" customWidth="1"/>
-    <col min="9730" max="9730" width="22.88671875" customWidth="1"/>
-    <col min="9732" max="9732" width="5.5546875" customWidth="1"/>
-    <col min="9733" max="9733" width="14.44140625" customWidth="1"/>
-    <col min="9986" max="9986" width="22.88671875" customWidth="1"/>
-    <col min="9988" max="9988" width="5.5546875" customWidth="1"/>
-    <col min="9989" max="9989" width="14.44140625" customWidth="1"/>
-    <col min="10242" max="10242" width="22.88671875" customWidth="1"/>
-    <col min="10244" max="10244" width="5.5546875" customWidth="1"/>
-    <col min="10245" max="10245" width="14.44140625" customWidth="1"/>
-    <col min="10498" max="10498" width="22.88671875" customWidth="1"/>
-    <col min="10500" max="10500" width="5.5546875" customWidth="1"/>
-    <col min="10501" max="10501" width="14.44140625" customWidth="1"/>
-    <col min="10754" max="10754" width="22.88671875" customWidth="1"/>
-    <col min="10756" max="10756" width="5.5546875" customWidth="1"/>
-    <col min="10757" max="10757" width="14.44140625" customWidth="1"/>
-    <col min="11010" max="11010" width="22.88671875" customWidth="1"/>
-    <col min="11012" max="11012" width="5.5546875" customWidth="1"/>
-    <col min="11013" max="11013" width="14.44140625" customWidth="1"/>
-    <col min="11266" max="11266" width="22.88671875" customWidth="1"/>
-    <col min="11268" max="11268" width="5.5546875" customWidth="1"/>
-    <col min="11269" max="11269" width="14.44140625" customWidth="1"/>
-    <col min="11522" max="11522" width="22.88671875" customWidth="1"/>
-    <col min="11524" max="11524" width="5.5546875" customWidth="1"/>
-    <col min="11525" max="11525" width="14.44140625" customWidth="1"/>
-    <col min="11778" max="11778" width="22.88671875" customWidth="1"/>
-    <col min="11780" max="11780" width="5.5546875" customWidth="1"/>
-    <col min="11781" max="11781" width="14.44140625" customWidth="1"/>
-    <col min="12034" max="12034" width="22.88671875" customWidth="1"/>
-    <col min="12036" max="12036" width="5.5546875" customWidth="1"/>
-    <col min="12037" max="12037" width="14.44140625" customWidth="1"/>
-    <col min="12290" max="12290" width="22.88671875" customWidth="1"/>
-    <col min="12292" max="12292" width="5.5546875" customWidth="1"/>
-    <col min="12293" max="12293" width="14.44140625" customWidth="1"/>
-    <col min="12546" max="12546" width="22.88671875" customWidth="1"/>
-    <col min="12548" max="12548" width="5.5546875" customWidth="1"/>
-    <col min="12549" max="12549" width="14.44140625" customWidth="1"/>
-    <col min="12802" max="12802" width="22.88671875" customWidth="1"/>
-    <col min="12804" max="12804" width="5.5546875" customWidth="1"/>
-    <col min="12805" max="12805" width="14.44140625" customWidth="1"/>
-    <col min="13058" max="13058" width="22.88671875" customWidth="1"/>
-    <col min="13060" max="13060" width="5.5546875" customWidth="1"/>
-    <col min="13061" max="13061" width="14.44140625" customWidth="1"/>
-    <col min="13314" max="13314" width="22.88671875" customWidth="1"/>
-    <col min="13316" max="13316" width="5.5546875" customWidth="1"/>
-    <col min="13317" max="13317" width="14.44140625" customWidth="1"/>
-    <col min="13570" max="13570" width="22.88671875" customWidth="1"/>
-    <col min="13572" max="13572" width="5.5546875" customWidth="1"/>
-    <col min="13573" max="13573" width="14.44140625" customWidth="1"/>
-    <col min="13826" max="13826" width="22.88671875" customWidth="1"/>
-    <col min="13828" max="13828" width="5.5546875" customWidth="1"/>
-    <col min="13829" max="13829" width="14.44140625" customWidth="1"/>
-    <col min="14082" max="14082" width="22.88671875" customWidth="1"/>
-    <col min="14084" max="14084" width="5.5546875" customWidth="1"/>
-    <col min="14085" max="14085" width="14.44140625" customWidth="1"/>
-    <col min="14338" max="14338" width="22.88671875" customWidth="1"/>
-    <col min="14340" max="14340" width="5.5546875" customWidth="1"/>
-    <col min="14341" max="14341" width="14.44140625" customWidth="1"/>
-    <col min="14594" max="14594" width="22.88671875" customWidth="1"/>
-    <col min="14596" max="14596" width="5.5546875" customWidth="1"/>
-    <col min="14597" max="14597" width="14.44140625" customWidth="1"/>
-    <col min="14850" max="14850" width="22.88671875" customWidth="1"/>
-    <col min="14852" max="14852" width="5.5546875" customWidth="1"/>
-    <col min="14853" max="14853" width="14.44140625" customWidth="1"/>
-    <col min="15106" max="15106" width="22.88671875" customWidth="1"/>
-    <col min="15108" max="15108" width="5.5546875" customWidth="1"/>
-    <col min="15109" max="15109" width="14.44140625" customWidth="1"/>
-    <col min="15362" max="15362" width="22.88671875" customWidth="1"/>
-    <col min="15364" max="15364" width="5.5546875" customWidth="1"/>
-    <col min="15365" max="15365" width="14.44140625" customWidth="1"/>
-    <col min="15618" max="15618" width="22.88671875" customWidth="1"/>
-    <col min="15620" max="15620" width="5.5546875" customWidth="1"/>
-    <col min="15621" max="15621" width="14.44140625" customWidth="1"/>
-    <col min="15874" max="15874" width="22.88671875" customWidth="1"/>
-    <col min="15876" max="15876" width="5.5546875" customWidth="1"/>
-    <col min="15877" max="15877" width="14.44140625" customWidth="1"/>
-    <col min="16130" max="16130" width="22.88671875" customWidth="1"/>
-    <col min="16132" max="16132" width="5.5546875" customWidth="1"/>
-    <col min="16133" max="16133" width="14.44140625" customWidth="1"/>
+    <col min="2" max="2" width="22.83203125" style="14" customWidth="1"/>
+    <col min="4" max="4" width="5.5" customWidth="1"/>
+    <col min="5" max="5" width="14.5" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" customWidth="1"/>
+    <col min="258" max="258" width="22.83203125" customWidth="1"/>
+    <col min="260" max="260" width="5.5" customWidth="1"/>
+    <col min="261" max="261" width="14.5" customWidth="1"/>
+    <col min="514" max="514" width="22.83203125" customWidth="1"/>
+    <col min="516" max="516" width="5.5" customWidth="1"/>
+    <col min="517" max="517" width="14.5" customWidth="1"/>
+    <col min="770" max="770" width="22.83203125" customWidth="1"/>
+    <col min="772" max="772" width="5.5" customWidth="1"/>
+    <col min="773" max="773" width="14.5" customWidth="1"/>
+    <col min="1026" max="1026" width="22.83203125" customWidth="1"/>
+    <col min="1028" max="1028" width="5.5" customWidth="1"/>
+    <col min="1029" max="1029" width="14.5" customWidth="1"/>
+    <col min="1282" max="1282" width="22.83203125" customWidth="1"/>
+    <col min="1284" max="1284" width="5.5" customWidth="1"/>
+    <col min="1285" max="1285" width="14.5" customWidth="1"/>
+    <col min="1538" max="1538" width="22.83203125" customWidth="1"/>
+    <col min="1540" max="1540" width="5.5" customWidth="1"/>
+    <col min="1541" max="1541" width="14.5" customWidth="1"/>
+    <col min="1794" max="1794" width="22.83203125" customWidth="1"/>
+    <col min="1796" max="1796" width="5.5" customWidth="1"/>
+    <col min="1797" max="1797" width="14.5" customWidth="1"/>
+    <col min="2050" max="2050" width="22.83203125" customWidth="1"/>
+    <col min="2052" max="2052" width="5.5" customWidth="1"/>
+    <col min="2053" max="2053" width="14.5" customWidth="1"/>
+    <col min="2306" max="2306" width="22.83203125" customWidth="1"/>
+    <col min="2308" max="2308" width="5.5" customWidth="1"/>
+    <col min="2309" max="2309" width="14.5" customWidth="1"/>
+    <col min="2562" max="2562" width="22.83203125" customWidth="1"/>
+    <col min="2564" max="2564" width="5.5" customWidth="1"/>
+    <col min="2565" max="2565" width="14.5" customWidth="1"/>
+    <col min="2818" max="2818" width="22.83203125" customWidth="1"/>
+    <col min="2820" max="2820" width="5.5" customWidth="1"/>
+    <col min="2821" max="2821" width="14.5" customWidth="1"/>
+    <col min="3074" max="3074" width="22.83203125" customWidth="1"/>
+    <col min="3076" max="3076" width="5.5" customWidth="1"/>
+    <col min="3077" max="3077" width="14.5" customWidth="1"/>
+    <col min="3330" max="3330" width="22.83203125" customWidth="1"/>
+    <col min="3332" max="3332" width="5.5" customWidth="1"/>
+    <col min="3333" max="3333" width="14.5" customWidth="1"/>
+    <col min="3586" max="3586" width="22.83203125" customWidth="1"/>
+    <col min="3588" max="3588" width="5.5" customWidth="1"/>
+    <col min="3589" max="3589" width="14.5" customWidth="1"/>
+    <col min="3842" max="3842" width="22.83203125" customWidth="1"/>
+    <col min="3844" max="3844" width="5.5" customWidth="1"/>
+    <col min="3845" max="3845" width="14.5" customWidth="1"/>
+    <col min="4098" max="4098" width="22.83203125" customWidth="1"/>
+    <col min="4100" max="4100" width="5.5" customWidth="1"/>
+    <col min="4101" max="4101" width="14.5" customWidth="1"/>
+    <col min="4354" max="4354" width="22.83203125" customWidth="1"/>
+    <col min="4356" max="4356" width="5.5" customWidth="1"/>
+    <col min="4357" max="4357" width="14.5" customWidth="1"/>
+    <col min="4610" max="4610" width="22.83203125" customWidth="1"/>
+    <col min="4612" max="4612" width="5.5" customWidth="1"/>
+    <col min="4613" max="4613" width="14.5" customWidth="1"/>
+    <col min="4866" max="4866" width="22.83203125" customWidth="1"/>
+    <col min="4868" max="4868" width="5.5" customWidth="1"/>
+    <col min="4869" max="4869" width="14.5" customWidth="1"/>
+    <col min="5122" max="5122" width="22.83203125" customWidth="1"/>
+    <col min="5124" max="5124" width="5.5" customWidth="1"/>
+    <col min="5125" max="5125" width="14.5" customWidth="1"/>
+    <col min="5378" max="5378" width="22.83203125" customWidth="1"/>
+    <col min="5380" max="5380" width="5.5" customWidth="1"/>
+    <col min="5381" max="5381" width="14.5" customWidth="1"/>
+    <col min="5634" max="5634" width="22.83203125" customWidth="1"/>
+    <col min="5636" max="5636" width="5.5" customWidth="1"/>
+    <col min="5637" max="5637" width="14.5" customWidth="1"/>
+    <col min="5890" max="5890" width="22.83203125" customWidth="1"/>
+    <col min="5892" max="5892" width="5.5" customWidth="1"/>
+    <col min="5893" max="5893" width="14.5" customWidth="1"/>
+    <col min="6146" max="6146" width="22.83203125" customWidth="1"/>
+    <col min="6148" max="6148" width="5.5" customWidth="1"/>
+    <col min="6149" max="6149" width="14.5" customWidth="1"/>
+    <col min="6402" max="6402" width="22.83203125" customWidth="1"/>
+    <col min="6404" max="6404" width="5.5" customWidth="1"/>
+    <col min="6405" max="6405" width="14.5" customWidth="1"/>
+    <col min="6658" max="6658" width="22.83203125" customWidth="1"/>
+    <col min="6660" max="6660" width="5.5" customWidth="1"/>
+    <col min="6661" max="6661" width="14.5" customWidth="1"/>
+    <col min="6914" max="6914" width="22.83203125" customWidth="1"/>
+    <col min="6916" max="6916" width="5.5" customWidth="1"/>
+    <col min="6917" max="6917" width="14.5" customWidth="1"/>
+    <col min="7170" max="7170" width="22.83203125" customWidth="1"/>
+    <col min="7172" max="7172" width="5.5" customWidth="1"/>
+    <col min="7173" max="7173" width="14.5" customWidth="1"/>
+    <col min="7426" max="7426" width="22.83203125" customWidth="1"/>
+    <col min="7428" max="7428" width="5.5" customWidth="1"/>
+    <col min="7429" max="7429" width="14.5" customWidth="1"/>
+    <col min="7682" max="7682" width="22.83203125" customWidth="1"/>
+    <col min="7684" max="7684" width="5.5" customWidth="1"/>
+    <col min="7685" max="7685" width="14.5" customWidth="1"/>
+    <col min="7938" max="7938" width="22.83203125" customWidth="1"/>
+    <col min="7940" max="7940" width="5.5" customWidth="1"/>
+    <col min="7941" max="7941" width="14.5" customWidth="1"/>
+    <col min="8194" max="8194" width="22.83203125" customWidth="1"/>
+    <col min="8196" max="8196" width="5.5" customWidth="1"/>
+    <col min="8197" max="8197" width="14.5" customWidth="1"/>
+    <col min="8450" max="8450" width="22.83203125" customWidth="1"/>
+    <col min="8452" max="8452" width="5.5" customWidth="1"/>
+    <col min="8453" max="8453" width="14.5" customWidth="1"/>
+    <col min="8706" max="8706" width="22.83203125" customWidth="1"/>
+    <col min="8708" max="8708" width="5.5" customWidth="1"/>
+    <col min="8709" max="8709" width="14.5" customWidth="1"/>
+    <col min="8962" max="8962" width="22.83203125" customWidth="1"/>
+    <col min="8964" max="8964" width="5.5" customWidth="1"/>
+    <col min="8965" max="8965" width="14.5" customWidth="1"/>
+    <col min="9218" max="9218" width="22.83203125" customWidth="1"/>
+    <col min="9220" max="9220" width="5.5" customWidth="1"/>
+    <col min="9221" max="9221" width="14.5" customWidth="1"/>
+    <col min="9474" max="9474" width="22.83203125" customWidth="1"/>
+    <col min="9476" max="9476" width="5.5" customWidth="1"/>
+    <col min="9477" max="9477" width="14.5" customWidth="1"/>
+    <col min="9730" max="9730" width="22.83203125" customWidth="1"/>
+    <col min="9732" max="9732" width="5.5" customWidth="1"/>
+    <col min="9733" max="9733" width="14.5" customWidth="1"/>
+    <col min="9986" max="9986" width="22.83203125" customWidth="1"/>
+    <col min="9988" max="9988" width="5.5" customWidth="1"/>
+    <col min="9989" max="9989" width="14.5" customWidth="1"/>
+    <col min="10242" max="10242" width="22.83203125" customWidth="1"/>
+    <col min="10244" max="10244" width="5.5" customWidth="1"/>
+    <col min="10245" max="10245" width="14.5" customWidth="1"/>
+    <col min="10498" max="10498" width="22.83203125" customWidth="1"/>
+    <col min="10500" max="10500" width="5.5" customWidth="1"/>
+    <col min="10501" max="10501" width="14.5" customWidth="1"/>
+    <col min="10754" max="10754" width="22.83203125" customWidth="1"/>
+    <col min="10756" max="10756" width="5.5" customWidth="1"/>
+    <col min="10757" max="10757" width="14.5" customWidth="1"/>
+    <col min="11010" max="11010" width="22.83203125" customWidth="1"/>
+    <col min="11012" max="11012" width="5.5" customWidth="1"/>
+    <col min="11013" max="11013" width="14.5" customWidth="1"/>
+    <col min="11266" max="11266" width="22.83203125" customWidth="1"/>
+    <col min="11268" max="11268" width="5.5" customWidth="1"/>
+    <col min="11269" max="11269" width="14.5" customWidth="1"/>
+    <col min="11522" max="11522" width="22.83203125" customWidth="1"/>
+    <col min="11524" max="11524" width="5.5" customWidth="1"/>
+    <col min="11525" max="11525" width="14.5" customWidth="1"/>
+    <col min="11778" max="11778" width="22.83203125" customWidth="1"/>
+    <col min="11780" max="11780" width="5.5" customWidth="1"/>
+    <col min="11781" max="11781" width="14.5" customWidth="1"/>
+    <col min="12034" max="12034" width="22.83203125" customWidth="1"/>
+    <col min="12036" max="12036" width="5.5" customWidth="1"/>
+    <col min="12037" max="12037" width="14.5" customWidth="1"/>
+    <col min="12290" max="12290" width="22.83203125" customWidth="1"/>
+    <col min="12292" max="12292" width="5.5" customWidth="1"/>
+    <col min="12293" max="12293" width="14.5" customWidth="1"/>
+    <col min="12546" max="12546" width="22.83203125" customWidth="1"/>
+    <col min="12548" max="12548" width="5.5" customWidth="1"/>
+    <col min="12549" max="12549" width="14.5" customWidth="1"/>
+    <col min="12802" max="12802" width="22.83203125" customWidth="1"/>
+    <col min="12804" max="12804" width="5.5" customWidth="1"/>
+    <col min="12805" max="12805" width="14.5" customWidth="1"/>
+    <col min="13058" max="13058" width="22.83203125" customWidth="1"/>
+    <col min="13060" max="13060" width="5.5" customWidth="1"/>
+    <col min="13061" max="13061" width="14.5" customWidth="1"/>
+    <col min="13314" max="13314" width="22.83203125" customWidth="1"/>
+    <col min="13316" max="13316" width="5.5" customWidth="1"/>
+    <col min="13317" max="13317" width="14.5" customWidth="1"/>
+    <col min="13570" max="13570" width="22.83203125" customWidth="1"/>
+    <col min="13572" max="13572" width="5.5" customWidth="1"/>
+    <col min="13573" max="13573" width="14.5" customWidth="1"/>
+    <col min="13826" max="13826" width="22.83203125" customWidth="1"/>
+    <col min="13828" max="13828" width="5.5" customWidth="1"/>
+    <col min="13829" max="13829" width="14.5" customWidth="1"/>
+    <col min="14082" max="14082" width="22.83203125" customWidth="1"/>
+    <col min="14084" max="14084" width="5.5" customWidth="1"/>
+    <col min="14085" max="14085" width="14.5" customWidth="1"/>
+    <col min="14338" max="14338" width="22.83203125" customWidth="1"/>
+    <col min="14340" max="14340" width="5.5" customWidth="1"/>
+    <col min="14341" max="14341" width="14.5" customWidth="1"/>
+    <col min="14594" max="14594" width="22.83203125" customWidth="1"/>
+    <col min="14596" max="14596" width="5.5" customWidth="1"/>
+    <col min="14597" max="14597" width="14.5" customWidth="1"/>
+    <col min="14850" max="14850" width="22.83203125" customWidth="1"/>
+    <col min="14852" max="14852" width="5.5" customWidth="1"/>
+    <col min="14853" max="14853" width="14.5" customWidth="1"/>
+    <col min="15106" max="15106" width="22.83203125" customWidth="1"/>
+    <col min="15108" max="15108" width="5.5" customWidth="1"/>
+    <col min="15109" max="15109" width="14.5" customWidth="1"/>
+    <col min="15362" max="15362" width="22.83203125" customWidth="1"/>
+    <col min="15364" max="15364" width="5.5" customWidth="1"/>
+    <col min="15365" max="15365" width="14.5" customWidth="1"/>
+    <col min="15618" max="15618" width="22.83203125" customWidth="1"/>
+    <col min="15620" max="15620" width="5.5" customWidth="1"/>
+    <col min="15621" max="15621" width="14.5" customWidth="1"/>
+    <col min="15874" max="15874" width="22.83203125" customWidth="1"/>
+    <col min="15876" max="15876" width="5.5" customWidth="1"/>
+    <col min="15877" max="15877" width="14.5" customWidth="1"/>
+    <col min="16130" max="16130" width="22.83203125" customWidth="1"/>
+    <col min="16132" max="16132" width="5.5" customWidth="1"/>
+    <col min="16133" max="16133" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
-      <c r="B4" s="62" t="s">
+      <c r="B4" s="49" t="s">
         <v>149</v>
       </c>
-      <c r="C4" s="62"/>
-      <c r="D4" s="62"/>
-      <c r="E4" s="62"/>
-      <c r="F4" s="62"/>
-      <c r="G4" s="62"/>
-      <c r="H4" s="62"/>
-      <c r="I4" s="62"/>
-      <c r="J4" s="62"/>
-      <c r="K4" s="62"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="49"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
-      <c r="B5" s="62" t="s">
+      <c r="B5" s="49" t="s">
         <v>152</v>
       </c>
-      <c r="C5" s="62"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="62"/>
-      <c r="H5" s="62"/>
-      <c r="I5" s="62"/>
-      <c r="J5" s="62"/>
-      <c r="K5" s="62"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="49"/>
+      <c r="J5" s="49"/>
+      <c r="K5" s="49"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
-      <c r="B6" s="63" t="s">
+      <c r="B6" s="50" t="s">
         <v>150</v>
       </c>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="63"/>
-      <c r="G6" s="63"/>
-      <c r="H6" s="63"/>
-      <c r="I6" s="63"/>
-      <c r="J6" s="63"/>
-      <c r="K6" s="63"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="50"/>
+      <c r="I6" s="50"/>
+      <c r="J6" s="50"/>
+      <c r="K6" s="50"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="64">
+      <c r="C9" s="51">
         <v>12</v>
       </c>
-      <c r="E9" s="34" t="s">
+      <c r="E9" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B10" s="18" t="s">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B10" s="14" t="s">
         <v>29</v>
       </c>
       <c r="C10">
@@ -2478,108 +2457,108 @@
         <v>8.3333333333333338E-8</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B11" s="18" t="s">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B11" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="65">
+      <c r="C11" s="52">
         <v>24</v>
       </c>
       <c r="E11" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B12" s="18" t="s">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B12" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="66">
-        <v>2</v>
+      <c r="C12" s="53">
+        <v>1</v>
       </c>
       <c r="E12" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B13" s="18" t="s">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B13" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="C13" s="77">
+      <c r="C13" s="64">
         <f>C10*(16+8*C12)</f>
-        <v>2.6666666666666668E-6</v>
+        <v>2.0000000000000003E-6</v>
       </c>
       <c r="E13" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="C14" s="21"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B15" s="18" t="s">
+      <c r="C14" s="19"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B15" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="67">
-        <v>7.4999999999999997E-3</v>
-      </c>
-      <c r="D15" s="21"/>
+      <c r="C15" s="54">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D15" s="19"/>
       <c r="E15" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B16" s="18" t="s">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B16" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="68">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B17" s="18" t="s">
+      <c r="C16" s="55">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B17" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="66">
-        <v>1.4139999999999999</v>
+      <c r="C17" s="53">
+        <v>0.47499999999999998</v>
       </c>
       <c r="E17" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B18" s="18" t="s">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B18" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="46">
+      <c r="C18" s="20">
         <f>C17/SQRT(2)</f>
-        <v>0.99984898859777804</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+        <v>0.33587572106361002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="C19" s="46"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B20" s="18" t="s">
+      <c r="C19" s="20"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B20" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="84">
+      <c r="C20" s="71">
         <v>3</v>
       </c>
       <c r="E20" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B21" s="18" t="s">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B21" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="77">
+      <c r="C21" s="64">
         <f>(24+32*C20)*C10</f>
         <v>1.0000000000000001E-5</v>
       </c>
@@ -2587,81 +2566,81 @@
         <v>121</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B23" s="18" t="s">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B23" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="C23" s="22">
+      <c r="C23" s="20">
         <f>C11*0.0000002/C15</f>
-        <v>6.3999999999999994E-4</v>
+        <v>7.9999999999999993E-4</v>
       </c>
       <c r="E23" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B24" s="18" t="s">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B24" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C24" s="22">
+      <c r="C24" s="20">
         <f>C11*C13/C15</f>
-        <v>8.5333333333333355E-3</v>
+        <v>8.0000000000000019E-3</v>
       </c>
       <c r="E24" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B25" s="18" t="s">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B25" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="22">
+      <c r="C25" s="20">
         <f>C16*C17*2*C21/C15</f>
-        <v>1.6968E-2</v>
+        <v>1.5833333333333335E-2</v>
       </c>
       <c r="E25" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B27" s="18" t="s">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B27" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="C27" s="84">
-        <v>31</v>
+      <c r="C27" s="71">
+        <v>10</v>
       </c>
       <c r="E27" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B28" s="18" t="s">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B28" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C28" s="23" t="str">
+      <c r="C28" s="21" t="str">
         <f>IF(C27&lt;16,"Current scaler is quite small - values above 16 are best for good microstepping","OK")</f>
-        <v>OK</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A29" s="42" t="s">
+        <v>Current scaler is quite small - values above 16 are best for good microstepping</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="B29" s="43"/>
-      <c r="C29" s="44"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="45"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B30" s="14" t="s">
+      <c r="B29" s="34"/>
+      <c r="C29" s="35"/>
+      <c r="D29" s="36"/>
+      <c r="E29" s="36"/>
+      <c r="F29" s="36"/>
+      <c r="G29" s="36"/>
+      <c r="H29" s="36"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B30" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="C30" s="41">
+      <c r="C30" s="32">
         <f>MAX(0.5+(C23+C24+C25)*2*248*(C27+1)/C17/32-8,-2)</f>
-        <v>1.6698029231494598</v>
+        <v>1.3420701754385984</v>
       </c>
       <c r="E30" t="s">
         <v>130</v>
@@ -2670,178 +2649,178 @@
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="J31" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A32" s="19" t="s">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="C32" s="24" t="s">
+      <c r="C32" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="F32" s="69" t="s">
+      <c r="F32" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="G32" s="70"/>
-      <c r="H32" s="71"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B33" s="37" t="s">
+      <c r="G32" s="57"/>
+      <c r="H32" s="58"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B33" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="C33" s="25">
+      <c r="C33" s="23">
         <f>MAX(MIN(C30,8),1)</f>
-        <v>1.6698029231494598</v>
+        <v>1.3420701754385984</v>
       </c>
       <c r="E33" t="s">
         <v>47</v>
       </c>
-      <c r="F33" s="72">
+      <c r="F33" s="59">
         <f>C33-1</f>
-        <v>0.66980292314945977</v>
-      </c>
-      <c r="G33" s="57" t="s">
+        <v>0.34207017543859841</v>
+      </c>
+      <c r="G33" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="H33" s="73"/>
+      <c r="H33" s="60"/>
       <c r="I33" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="37" t="s">
+    <row r="34" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="30" t="s">
         <v>102</v>
       </c>
-      <c r="C34" s="25">
+      <c r="C34" s="23">
         <f>MIN(C30-C33,12)</f>
         <v>0</v>
       </c>
       <c r="E34" t="s">
         <v>48</v>
       </c>
-      <c r="F34" s="74">
+      <c r="F34" s="61">
         <f>C34+3</f>
         <v>3</v>
       </c>
-      <c r="G34" s="75" t="s">
+      <c r="G34" s="62" t="s">
         <v>100</v>
       </c>
-      <c r="H34" s="76"/>
+      <c r="H34" s="63"/>
       <c r="I34" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B36" s="18" t="s">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B36" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C36" s="23" t="str">
+      <c r="C36" s="21" t="str">
         <f>IF(C30&gt;20,"Attention: Motor requires very high Hysteresis setting  - try with reduced setting, reduce tBLANK, reduce sense resistor valule, increase fCLK, decrease VM or use classic const_toff_chopper mode", IF(C30&gt;15, "Attention: Result is large, use with CS reduced to maximum 30, or try smaller value of 16","OK"))</f>
         <v>OK</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C37" s="23"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B38" s="18" t="s">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C37" s="21"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B38" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="C38" s="36">
+      <c r="C38" s="29">
         <f>1/(2*C21+2*C13)/1000</f>
-        <v>39.473684210526315</v>
+        <v>41.666666666666664</v>
       </c>
       <c r="E38" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B39" s="18" t="s">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B39" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C39" s="23" t="str">
+      <c r="C39" s="21" t="str">
         <f>IF(C38&gt;50,"Attention: Motor frequency might get quite high - work with increased hysteresis setting and measure actual frequency, or use ChopSync",IF(C38&lt;20,"The chopper frequency is low and might become audible - increase slow decay time tOFF","OK"))</f>
         <v>OK</v>
       </c>
-      <c r="H39" s="16"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B41" s="18" t="s">
+      <c r="H39" s="15"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B41" s="14" t="s">
         <v>50</v>
       </c>
       <c r="C41" s="3">
         <f>C16*C17/SQRT(2)</f>
-        <v>4.4993204486900016</v>
+        <v>3.3587572106361003</v>
       </c>
       <c r="E41" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>117</v>
       </c>
       <c r="C42" s="3"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B43" s="18" t="s">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B43" s="14" t="s">
         <v>52</v>
       </c>
       <c r="C43" s="7">
         <f>20*C41</f>
-        <v>89.986408973800025</v>
-      </c>
-      <c r="E43" s="26" t="s">
+        <v>67.175144212722003</v>
+      </c>
+      <c r="E43" s="24" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B44" s="18" t="s">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B44" s="14" t="s">
         <v>54</v>
       </c>
       <c r="C44" s="7">
         <f>C41*2</f>
-        <v>8.9986408973800032</v>
+        <v>6.7175144212722007</v>
       </c>
       <c r="E44" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B45"/>
     </row>
-    <row r="46" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B47" s="80" t="s">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B47" s="67" t="s">
         <v>153</v>
       </c>
-      <c r="C47" s="78">
+      <c r="C47" s="65">
         <f>(C27+1)/32/C17*0.32-0.02</f>
-        <v>0.20630834512022633</v>
-      </c>
-      <c r="D47" s="81" t="s">
+        <v>0.21157894736842109</v>
+      </c>
+      <c r="D47" s="68" t="s">
         <v>56</v>
       </c>
       <c r="E47" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B48" s="82" t="s">
+    <row r="48" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="69" t="s">
         <v>154</v>
       </c>
-      <c r="C48" s="79">
+      <c r="C48" s="66">
         <f>(C27+1)/32/C17*0.18-0.02</f>
-        <v>0.10729844413012728</v>
-      </c>
-      <c r="D48" s="83" t="s">
+        <v>0.11026315789473683</v>
+      </c>
+      <c r="D48" s="70" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2869,393 +2848,393 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="39.88671875" customWidth="1"/>
-    <col min="2" max="2" width="23.109375" customWidth="1"/>
-    <col min="3" max="3" width="16.88671875" customWidth="1"/>
-    <col min="4" max="4" width="17.44140625" customWidth="1"/>
-    <col min="5" max="5" width="17.109375" customWidth="1"/>
-    <col min="257" max="257" width="39.88671875" customWidth="1"/>
-    <col min="258" max="258" width="23.109375" customWidth="1"/>
-    <col min="259" max="259" width="16.88671875" customWidth="1"/>
-    <col min="260" max="260" width="17.44140625" customWidth="1"/>
-    <col min="261" max="261" width="17.109375" customWidth="1"/>
-    <col min="513" max="513" width="39.88671875" customWidth="1"/>
-    <col min="514" max="514" width="23.109375" customWidth="1"/>
-    <col min="515" max="515" width="16.88671875" customWidth="1"/>
-    <col min="516" max="516" width="17.44140625" customWidth="1"/>
-    <col min="517" max="517" width="17.109375" customWidth="1"/>
-    <col min="769" max="769" width="39.88671875" customWidth="1"/>
-    <col min="770" max="770" width="23.109375" customWidth="1"/>
-    <col min="771" max="771" width="16.88671875" customWidth="1"/>
-    <col min="772" max="772" width="17.44140625" customWidth="1"/>
-    <col min="773" max="773" width="17.109375" customWidth="1"/>
-    <col min="1025" max="1025" width="39.88671875" customWidth="1"/>
-    <col min="1026" max="1026" width="23.109375" customWidth="1"/>
-    <col min="1027" max="1027" width="16.88671875" customWidth="1"/>
-    <col min="1028" max="1028" width="17.44140625" customWidth="1"/>
-    <col min="1029" max="1029" width="17.109375" customWidth="1"/>
-    <col min="1281" max="1281" width="39.88671875" customWidth="1"/>
-    <col min="1282" max="1282" width="23.109375" customWidth="1"/>
-    <col min="1283" max="1283" width="16.88671875" customWidth="1"/>
-    <col min="1284" max="1284" width="17.44140625" customWidth="1"/>
-    <col min="1285" max="1285" width="17.109375" customWidth="1"/>
-    <col min="1537" max="1537" width="39.88671875" customWidth="1"/>
-    <col min="1538" max="1538" width="23.109375" customWidth="1"/>
-    <col min="1539" max="1539" width="16.88671875" customWidth="1"/>
-    <col min="1540" max="1540" width="17.44140625" customWidth="1"/>
-    <col min="1541" max="1541" width="17.109375" customWidth="1"/>
-    <col min="1793" max="1793" width="39.88671875" customWidth="1"/>
-    <col min="1794" max="1794" width="23.109375" customWidth="1"/>
-    <col min="1795" max="1795" width="16.88671875" customWidth="1"/>
-    <col min="1796" max="1796" width="17.44140625" customWidth="1"/>
-    <col min="1797" max="1797" width="17.109375" customWidth="1"/>
-    <col min="2049" max="2049" width="39.88671875" customWidth="1"/>
-    <col min="2050" max="2050" width="23.109375" customWidth="1"/>
-    <col min="2051" max="2051" width="16.88671875" customWidth="1"/>
-    <col min="2052" max="2052" width="17.44140625" customWidth="1"/>
-    <col min="2053" max="2053" width="17.109375" customWidth="1"/>
-    <col min="2305" max="2305" width="39.88671875" customWidth="1"/>
-    <col min="2306" max="2306" width="23.109375" customWidth="1"/>
-    <col min="2307" max="2307" width="16.88671875" customWidth="1"/>
-    <col min="2308" max="2308" width="17.44140625" customWidth="1"/>
-    <col min="2309" max="2309" width="17.109375" customWidth="1"/>
-    <col min="2561" max="2561" width="39.88671875" customWidth="1"/>
-    <col min="2562" max="2562" width="23.109375" customWidth="1"/>
-    <col min="2563" max="2563" width="16.88671875" customWidth="1"/>
-    <col min="2564" max="2564" width="17.44140625" customWidth="1"/>
-    <col min="2565" max="2565" width="17.109375" customWidth="1"/>
-    <col min="2817" max="2817" width="39.88671875" customWidth="1"/>
-    <col min="2818" max="2818" width="23.109375" customWidth="1"/>
-    <col min="2819" max="2819" width="16.88671875" customWidth="1"/>
-    <col min="2820" max="2820" width="17.44140625" customWidth="1"/>
-    <col min="2821" max="2821" width="17.109375" customWidth="1"/>
-    <col min="3073" max="3073" width="39.88671875" customWidth="1"/>
-    <col min="3074" max="3074" width="23.109375" customWidth="1"/>
-    <col min="3075" max="3075" width="16.88671875" customWidth="1"/>
-    <col min="3076" max="3076" width="17.44140625" customWidth="1"/>
-    <col min="3077" max="3077" width="17.109375" customWidth="1"/>
-    <col min="3329" max="3329" width="39.88671875" customWidth="1"/>
-    <col min="3330" max="3330" width="23.109375" customWidth="1"/>
-    <col min="3331" max="3331" width="16.88671875" customWidth="1"/>
-    <col min="3332" max="3332" width="17.44140625" customWidth="1"/>
-    <col min="3333" max="3333" width="17.109375" customWidth="1"/>
-    <col min="3585" max="3585" width="39.88671875" customWidth="1"/>
-    <col min="3586" max="3586" width="23.109375" customWidth="1"/>
-    <col min="3587" max="3587" width="16.88671875" customWidth="1"/>
-    <col min="3588" max="3588" width="17.44140625" customWidth="1"/>
-    <col min="3589" max="3589" width="17.109375" customWidth="1"/>
-    <col min="3841" max="3841" width="39.88671875" customWidth="1"/>
-    <col min="3842" max="3842" width="23.109375" customWidth="1"/>
-    <col min="3843" max="3843" width="16.88671875" customWidth="1"/>
-    <col min="3844" max="3844" width="17.44140625" customWidth="1"/>
-    <col min="3845" max="3845" width="17.109375" customWidth="1"/>
-    <col min="4097" max="4097" width="39.88671875" customWidth="1"/>
-    <col min="4098" max="4098" width="23.109375" customWidth="1"/>
-    <col min="4099" max="4099" width="16.88671875" customWidth="1"/>
-    <col min="4100" max="4100" width="17.44140625" customWidth="1"/>
-    <col min="4101" max="4101" width="17.109375" customWidth="1"/>
-    <col min="4353" max="4353" width="39.88671875" customWidth="1"/>
-    <col min="4354" max="4354" width="23.109375" customWidth="1"/>
-    <col min="4355" max="4355" width="16.88671875" customWidth="1"/>
-    <col min="4356" max="4356" width="17.44140625" customWidth="1"/>
-    <col min="4357" max="4357" width="17.109375" customWidth="1"/>
-    <col min="4609" max="4609" width="39.88671875" customWidth="1"/>
-    <col min="4610" max="4610" width="23.109375" customWidth="1"/>
-    <col min="4611" max="4611" width="16.88671875" customWidth="1"/>
-    <col min="4612" max="4612" width="17.44140625" customWidth="1"/>
-    <col min="4613" max="4613" width="17.109375" customWidth="1"/>
-    <col min="4865" max="4865" width="39.88671875" customWidth="1"/>
-    <col min="4866" max="4866" width="23.109375" customWidth="1"/>
-    <col min="4867" max="4867" width="16.88671875" customWidth="1"/>
-    <col min="4868" max="4868" width="17.44140625" customWidth="1"/>
-    <col min="4869" max="4869" width="17.109375" customWidth="1"/>
-    <col min="5121" max="5121" width="39.88671875" customWidth="1"/>
-    <col min="5122" max="5122" width="23.109375" customWidth="1"/>
-    <col min="5123" max="5123" width="16.88671875" customWidth="1"/>
-    <col min="5124" max="5124" width="17.44140625" customWidth="1"/>
-    <col min="5125" max="5125" width="17.109375" customWidth="1"/>
-    <col min="5377" max="5377" width="39.88671875" customWidth="1"/>
-    <col min="5378" max="5378" width="23.109375" customWidth="1"/>
-    <col min="5379" max="5379" width="16.88671875" customWidth="1"/>
-    <col min="5380" max="5380" width="17.44140625" customWidth="1"/>
-    <col min="5381" max="5381" width="17.109375" customWidth="1"/>
-    <col min="5633" max="5633" width="39.88671875" customWidth="1"/>
-    <col min="5634" max="5634" width="23.109375" customWidth="1"/>
-    <col min="5635" max="5635" width="16.88671875" customWidth="1"/>
-    <col min="5636" max="5636" width="17.44140625" customWidth="1"/>
-    <col min="5637" max="5637" width="17.109375" customWidth="1"/>
-    <col min="5889" max="5889" width="39.88671875" customWidth="1"/>
-    <col min="5890" max="5890" width="23.109375" customWidth="1"/>
-    <col min="5891" max="5891" width="16.88671875" customWidth="1"/>
-    <col min="5892" max="5892" width="17.44140625" customWidth="1"/>
-    <col min="5893" max="5893" width="17.109375" customWidth="1"/>
-    <col min="6145" max="6145" width="39.88671875" customWidth="1"/>
-    <col min="6146" max="6146" width="23.109375" customWidth="1"/>
-    <col min="6147" max="6147" width="16.88671875" customWidth="1"/>
-    <col min="6148" max="6148" width="17.44140625" customWidth="1"/>
-    <col min="6149" max="6149" width="17.109375" customWidth="1"/>
-    <col min="6401" max="6401" width="39.88671875" customWidth="1"/>
-    <col min="6402" max="6402" width="23.109375" customWidth="1"/>
-    <col min="6403" max="6403" width="16.88671875" customWidth="1"/>
-    <col min="6404" max="6404" width="17.44140625" customWidth="1"/>
-    <col min="6405" max="6405" width="17.109375" customWidth="1"/>
-    <col min="6657" max="6657" width="39.88671875" customWidth="1"/>
-    <col min="6658" max="6658" width="23.109375" customWidth="1"/>
-    <col min="6659" max="6659" width="16.88671875" customWidth="1"/>
-    <col min="6660" max="6660" width="17.44140625" customWidth="1"/>
-    <col min="6661" max="6661" width="17.109375" customWidth="1"/>
-    <col min="6913" max="6913" width="39.88671875" customWidth="1"/>
-    <col min="6914" max="6914" width="23.109375" customWidth="1"/>
-    <col min="6915" max="6915" width="16.88671875" customWidth="1"/>
-    <col min="6916" max="6916" width="17.44140625" customWidth="1"/>
-    <col min="6917" max="6917" width="17.109375" customWidth="1"/>
-    <col min="7169" max="7169" width="39.88671875" customWidth="1"/>
-    <col min="7170" max="7170" width="23.109375" customWidth="1"/>
-    <col min="7171" max="7171" width="16.88671875" customWidth="1"/>
-    <col min="7172" max="7172" width="17.44140625" customWidth="1"/>
-    <col min="7173" max="7173" width="17.109375" customWidth="1"/>
-    <col min="7425" max="7425" width="39.88671875" customWidth="1"/>
-    <col min="7426" max="7426" width="23.109375" customWidth="1"/>
-    <col min="7427" max="7427" width="16.88671875" customWidth="1"/>
-    <col min="7428" max="7428" width="17.44140625" customWidth="1"/>
-    <col min="7429" max="7429" width="17.109375" customWidth="1"/>
-    <col min="7681" max="7681" width="39.88671875" customWidth="1"/>
-    <col min="7682" max="7682" width="23.109375" customWidth="1"/>
-    <col min="7683" max="7683" width="16.88671875" customWidth="1"/>
-    <col min="7684" max="7684" width="17.44140625" customWidth="1"/>
-    <col min="7685" max="7685" width="17.109375" customWidth="1"/>
-    <col min="7937" max="7937" width="39.88671875" customWidth="1"/>
-    <col min="7938" max="7938" width="23.109375" customWidth="1"/>
-    <col min="7939" max="7939" width="16.88671875" customWidth="1"/>
-    <col min="7940" max="7940" width="17.44140625" customWidth="1"/>
-    <col min="7941" max="7941" width="17.109375" customWidth="1"/>
-    <col min="8193" max="8193" width="39.88671875" customWidth="1"/>
-    <col min="8194" max="8194" width="23.109375" customWidth="1"/>
-    <col min="8195" max="8195" width="16.88671875" customWidth="1"/>
-    <col min="8196" max="8196" width="17.44140625" customWidth="1"/>
-    <col min="8197" max="8197" width="17.109375" customWidth="1"/>
-    <col min="8449" max="8449" width="39.88671875" customWidth="1"/>
-    <col min="8450" max="8450" width="23.109375" customWidth="1"/>
-    <col min="8451" max="8451" width="16.88671875" customWidth="1"/>
-    <col min="8452" max="8452" width="17.44140625" customWidth="1"/>
-    <col min="8453" max="8453" width="17.109375" customWidth="1"/>
-    <col min="8705" max="8705" width="39.88671875" customWidth="1"/>
-    <col min="8706" max="8706" width="23.109375" customWidth="1"/>
-    <col min="8707" max="8707" width="16.88671875" customWidth="1"/>
-    <col min="8708" max="8708" width="17.44140625" customWidth="1"/>
-    <col min="8709" max="8709" width="17.109375" customWidth="1"/>
-    <col min="8961" max="8961" width="39.88671875" customWidth="1"/>
-    <col min="8962" max="8962" width="23.109375" customWidth="1"/>
-    <col min="8963" max="8963" width="16.88671875" customWidth="1"/>
-    <col min="8964" max="8964" width="17.44140625" customWidth="1"/>
-    <col min="8965" max="8965" width="17.109375" customWidth="1"/>
-    <col min="9217" max="9217" width="39.88671875" customWidth="1"/>
-    <col min="9218" max="9218" width="23.109375" customWidth="1"/>
-    <col min="9219" max="9219" width="16.88671875" customWidth="1"/>
-    <col min="9220" max="9220" width="17.44140625" customWidth="1"/>
-    <col min="9221" max="9221" width="17.109375" customWidth="1"/>
-    <col min="9473" max="9473" width="39.88671875" customWidth="1"/>
-    <col min="9474" max="9474" width="23.109375" customWidth="1"/>
-    <col min="9475" max="9475" width="16.88671875" customWidth="1"/>
-    <col min="9476" max="9476" width="17.44140625" customWidth="1"/>
-    <col min="9477" max="9477" width="17.109375" customWidth="1"/>
-    <col min="9729" max="9729" width="39.88671875" customWidth="1"/>
-    <col min="9730" max="9730" width="23.109375" customWidth="1"/>
-    <col min="9731" max="9731" width="16.88671875" customWidth="1"/>
-    <col min="9732" max="9732" width="17.44140625" customWidth="1"/>
-    <col min="9733" max="9733" width="17.109375" customWidth="1"/>
-    <col min="9985" max="9985" width="39.88671875" customWidth="1"/>
-    <col min="9986" max="9986" width="23.109375" customWidth="1"/>
-    <col min="9987" max="9987" width="16.88671875" customWidth="1"/>
-    <col min="9988" max="9988" width="17.44140625" customWidth="1"/>
-    <col min="9989" max="9989" width="17.109375" customWidth="1"/>
-    <col min="10241" max="10241" width="39.88671875" customWidth="1"/>
-    <col min="10242" max="10242" width="23.109375" customWidth="1"/>
-    <col min="10243" max="10243" width="16.88671875" customWidth="1"/>
-    <col min="10244" max="10244" width="17.44140625" customWidth="1"/>
-    <col min="10245" max="10245" width="17.109375" customWidth="1"/>
-    <col min="10497" max="10497" width="39.88671875" customWidth="1"/>
-    <col min="10498" max="10498" width="23.109375" customWidth="1"/>
-    <col min="10499" max="10499" width="16.88671875" customWidth="1"/>
-    <col min="10500" max="10500" width="17.44140625" customWidth="1"/>
-    <col min="10501" max="10501" width="17.109375" customWidth="1"/>
-    <col min="10753" max="10753" width="39.88671875" customWidth="1"/>
-    <col min="10754" max="10754" width="23.109375" customWidth="1"/>
-    <col min="10755" max="10755" width="16.88671875" customWidth="1"/>
-    <col min="10756" max="10756" width="17.44140625" customWidth="1"/>
-    <col min="10757" max="10757" width="17.109375" customWidth="1"/>
-    <col min="11009" max="11009" width="39.88671875" customWidth="1"/>
-    <col min="11010" max="11010" width="23.109375" customWidth="1"/>
-    <col min="11011" max="11011" width="16.88671875" customWidth="1"/>
-    <col min="11012" max="11012" width="17.44140625" customWidth="1"/>
-    <col min="11013" max="11013" width="17.109375" customWidth="1"/>
-    <col min="11265" max="11265" width="39.88671875" customWidth="1"/>
-    <col min="11266" max="11266" width="23.109375" customWidth="1"/>
-    <col min="11267" max="11267" width="16.88671875" customWidth="1"/>
-    <col min="11268" max="11268" width="17.44140625" customWidth="1"/>
-    <col min="11269" max="11269" width="17.109375" customWidth="1"/>
-    <col min="11521" max="11521" width="39.88671875" customWidth="1"/>
-    <col min="11522" max="11522" width="23.109375" customWidth="1"/>
-    <col min="11523" max="11523" width="16.88671875" customWidth="1"/>
-    <col min="11524" max="11524" width="17.44140625" customWidth="1"/>
-    <col min="11525" max="11525" width="17.109375" customWidth="1"/>
-    <col min="11777" max="11777" width="39.88671875" customWidth="1"/>
-    <col min="11778" max="11778" width="23.109375" customWidth="1"/>
-    <col min="11779" max="11779" width="16.88671875" customWidth="1"/>
-    <col min="11780" max="11780" width="17.44140625" customWidth="1"/>
-    <col min="11781" max="11781" width="17.109375" customWidth="1"/>
-    <col min="12033" max="12033" width="39.88671875" customWidth="1"/>
-    <col min="12034" max="12034" width="23.109375" customWidth="1"/>
-    <col min="12035" max="12035" width="16.88671875" customWidth="1"/>
-    <col min="12036" max="12036" width="17.44140625" customWidth="1"/>
-    <col min="12037" max="12037" width="17.109375" customWidth="1"/>
-    <col min="12289" max="12289" width="39.88671875" customWidth="1"/>
-    <col min="12290" max="12290" width="23.109375" customWidth="1"/>
-    <col min="12291" max="12291" width="16.88671875" customWidth="1"/>
-    <col min="12292" max="12292" width="17.44140625" customWidth="1"/>
-    <col min="12293" max="12293" width="17.109375" customWidth="1"/>
-    <col min="12545" max="12545" width="39.88671875" customWidth="1"/>
-    <col min="12546" max="12546" width="23.109375" customWidth="1"/>
-    <col min="12547" max="12547" width="16.88671875" customWidth="1"/>
-    <col min="12548" max="12548" width="17.44140625" customWidth="1"/>
-    <col min="12549" max="12549" width="17.109375" customWidth="1"/>
-    <col min="12801" max="12801" width="39.88671875" customWidth="1"/>
-    <col min="12802" max="12802" width="23.109375" customWidth="1"/>
-    <col min="12803" max="12803" width="16.88671875" customWidth="1"/>
-    <col min="12804" max="12804" width="17.44140625" customWidth="1"/>
-    <col min="12805" max="12805" width="17.109375" customWidth="1"/>
-    <col min="13057" max="13057" width="39.88671875" customWidth="1"/>
-    <col min="13058" max="13058" width="23.109375" customWidth="1"/>
-    <col min="13059" max="13059" width="16.88671875" customWidth="1"/>
-    <col min="13060" max="13060" width="17.44140625" customWidth="1"/>
-    <col min="13061" max="13061" width="17.109375" customWidth="1"/>
-    <col min="13313" max="13313" width="39.88671875" customWidth="1"/>
-    <col min="13314" max="13314" width="23.109375" customWidth="1"/>
-    <col min="13315" max="13315" width="16.88671875" customWidth="1"/>
-    <col min="13316" max="13316" width="17.44140625" customWidth="1"/>
-    <col min="13317" max="13317" width="17.109375" customWidth="1"/>
-    <col min="13569" max="13569" width="39.88671875" customWidth="1"/>
-    <col min="13570" max="13570" width="23.109375" customWidth="1"/>
-    <col min="13571" max="13571" width="16.88671875" customWidth="1"/>
-    <col min="13572" max="13572" width="17.44140625" customWidth="1"/>
-    <col min="13573" max="13573" width="17.109375" customWidth="1"/>
-    <col min="13825" max="13825" width="39.88671875" customWidth="1"/>
-    <col min="13826" max="13826" width="23.109375" customWidth="1"/>
-    <col min="13827" max="13827" width="16.88671875" customWidth="1"/>
-    <col min="13828" max="13828" width="17.44140625" customWidth="1"/>
-    <col min="13829" max="13829" width="17.109375" customWidth="1"/>
-    <col min="14081" max="14081" width="39.88671875" customWidth="1"/>
-    <col min="14082" max="14082" width="23.109375" customWidth="1"/>
-    <col min="14083" max="14083" width="16.88671875" customWidth="1"/>
-    <col min="14084" max="14084" width="17.44140625" customWidth="1"/>
-    <col min="14085" max="14085" width="17.109375" customWidth="1"/>
-    <col min="14337" max="14337" width="39.88671875" customWidth="1"/>
-    <col min="14338" max="14338" width="23.109375" customWidth="1"/>
-    <col min="14339" max="14339" width="16.88671875" customWidth="1"/>
-    <col min="14340" max="14340" width="17.44140625" customWidth="1"/>
-    <col min="14341" max="14341" width="17.109375" customWidth="1"/>
-    <col min="14593" max="14593" width="39.88671875" customWidth="1"/>
-    <col min="14594" max="14594" width="23.109375" customWidth="1"/>
-    <col min="14595" max="14595" width="16.88671875" customWidth="1"/>
-    <col min="14596" max="14596" width="17.44140625" customWidth="1"/>
-    <col min="14597" max="14597" width="17.109375" customWidth="1"/>
-    <col min="14849" max="14849" width="39.88671875" customWidth="1"/>
-    <col min="14850" max="14850" width="23.109375" customWidth="1"/>
-    <col min="14851" max="14851" width="16.88671875" customWidth="1"/>
-    <col min="14852" max="14852" width="17.44140625" customWidth="1"/>
-    <col min="14853" max="14853" width="17.109375" customWidth="1"/>
-    <col min="15105" max="15105" width="39.88671875" customWidth="1"/>
-    <col min="15106" max="15106" width="23.109375" customWidth="1"/>
-    <col min="15107" max="15107" width="16.88671875" customWidth="1"/>
-    <col min="15108" max="15108" width="17.44140625" customWidth="1"/>
-    <col min="15109" max="15109" width="17.109375" customWidth="1"/>
-    <col min="15361" max="15361" width="39.88671875" customWidth="1"/>
-    <col min="15362" max="15362" width="23.109375" customWidth="1"/>
-    <col min="15363" max="15363" width="16.88671875" customWidth="1"/>
-    <col min="15364" max="15364" width="17.44140625" customWidth="1"/>
-    <col min="15365" max="15365" width="17.109375" customWidth="1"/>
-    <col min="15617" max="15617" width="39.88671875" customWidth="1"/>
-    <col min="15618" max="15618" width="23.109375" customWidth="1"/>
-    <col min="15619" max="15619" width="16.88671875" customWidth="1"/>
-    <col min="15620" max="15620" width="17.44140625" customWidth="1"/>
-    <col min="15621" max="15621" width="17.109375" customWidth="1"/>
-    <col min="15873" max="15873" width="39.88671875" customWidth="1"/>
-    <col min="15874" max="15874" width="23.109375" customWidth="1"/>
-    <col min="15875" max="15875" width="16.88671875" customWidth="1"/>
-    <col min="15876" max="15876" width="17.44140625" customWidth="1"/>
-    <col min="15877" max="15877" width="17.109375" customWidth="1"/>
-    <col min="16129" max="16129" width="39.88671875" customWidth="1"/>
-    <col min="16130" max="16130" width="23.109375" customWidth="1"/>
-    <col min="16131" max="16131" width="16.88671875" customWidth="1"/>
-    <col min="16132" max="16132" width="17.44140625" customWidth="1"/>
-    <col min="16133" max="16133" width="17.109375" customWidth="1"/>
+    <col min="1" max="1" width="39.83203125" customWidth="1"/>
+    <col min="2" max="2" width="23.1640625" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" customWidth="1"/>
+    <col min="4" max="4" width="17.5" customWidth="1"/>
+    <col min="5" max="5" width="17.1640625" customWidth="1"/>
+    <col min="257" max="257" width="39.83203125" customWidth="1"/>
+    <col min="258" max="258" width="23.1640625" customWidth="1"/>
+    <col min="259" max="259" width="16.83203125" customWidth="1"/>
+    <col min="260" max="260" width="17.5" customWidth="1"/>
+    <col min="261" max="261" width="17.1640625" customWidth="1"/>
+    <col min="513" max="513" width="39.83203125" customWidth="1"/>
+    <col min="514" max="514" width="23.1640625" customWidth="1"/>
+    <col min="515" max="515" width="16.83203125" customWidth="1"/>
+    <col min="516" max="516" width="17.5" customWidth="1"/>
+    <col min="517" max="517" width="17.1640625" customWidth="1"/>
+    <col min="769" max="769" width="39.83203125" customWidth="1"/>
+    <col min="770" max="770" width="23.1640625" customWidth="1"/>
+    <col min="771" max="771" width="16.83203125" customWidth="1"/>
+    <col min="772" max="772" width="17.5" customWidth="1"/>
+    <col min="773" max="773" width="17.1640625" customWidth="1"/>
+    <col min="1025" max="1025" width="39.83203125" customWidth="1"/>
+    <col min="1026" max="1026" width="23.1640625" customWidth="1"/>
+    <col min="1027" max="1027" width="16.83203125" customWidth="1"/>
+    <col min="1028" max="1028" width="17.5" customWidth="1"/>
+    <col min="1029" max="1029" width="17.1640625" customWidth="1"/>
+    <col min="1281" max="1281" width="39.83203125" customWidth="1"/>
+    <col min="1282" max="1282" width="23.1640625" customWidth="1"/>
+    <col min="1283" max="1283" width="16.83203125" customWidth="1"/>
+    <col min="1284" max="1284" width="17.5" customWidth="1"/>
+    <col min="1285" max="1285" width="17.1640625" customWidth="1"/>
+    <col min="1537" max="1537" width="39.83203125" customWidth="1"/>
+    <col min="1538" max="1538" width="23.1640625" customWidth="1"/>
+    <col min="1539" max="1539" width="16.83203125" customWidth="1"/>
+    <col min="1540" max="1540" width="17.5" customWidth="1"/>
+    <col min="1541" max="1541" width="17.1640625" customWidth="1"/>
+    <col min="1793" max="1793" width="39.83203125" customWidth="1"/>
+    <col min="1794" max="1794" width="23.1640625" customWidth="1"/>
+    <col min="1795" max="1795" width="16.83203125" customWidth="1"/>
+    <col min="1796" max="1796" width="17.5" customWidth="1"/>
+    <col min="1797" max="1797" width="17.1640625" customWidth="1"/>
+    <col min="2049" max="2049" width="39.83203125" customWidth="1"/>
+    <col min="2050" max="2050" width="23.1640625" customWidth="1"/>
+    <col min="2051" max="2051" width="16.83203125" customWidth="1"/>
+    <col min="2052" max="2052" width="17.5" customWidth="1"/>
+    <col min="2053" max="2053" width="17.1640625" customWidth="1"/>
+    <col min="2305" max="2305" width="39.83203125" customWidth="1"/>
+    <col min="2306" max="2306" width="23.1640625" customWidth="1"/>
+    <col min="2307" max="2307" width="16.83203125" customWidth="1"/>
+    <col min="2308" max="2308" width="17.5" customWidth="1"/>
+    <col min="2309" max="2309" width="17.1640625" customWidth="1"/>
+    <col min="2561" max="2561" width="39.83203125" customWidth="1"/>
+    <col min="2562" max="2562" width="23.1640625" customWidth="1"/>
+    <col min="2563" max="2563" width="16.83203125" customWidth="1"/>
+    <col min="2564" max="2564" width="17.5" customWidth="1"/>
+    <col min="2565" max="2565" width="17.1640625" customWidth="1"/>
+    <col min="2817" max="2817" width="39.83203125" customWidth="1"/>
+    <col min="2818" max="2818" width="23.1640625" customWidth="1"/>
+    <col min="2819" max="2819" width="16.83203125" customWidth="1"/>
+    <col min="2820" max="2820" width="17.5" customWidth="1"/>
+    <col min="2821" max="2821" width="17.1640625" customWidth="1"/>
+    <col min="3073" max="3073" width="39.83203125" customWidth="1"/>
+    <col min="3074" max="3074" width="23.1640625" customWidth="1"/>
+    <col min="3075" max="3075" width="16.83203125" customWidth="1"/>
+    <col min="3076" max="3076" width="17.5" customWidth="1"/>
+    <col min="3077" max="3077" width="17.1640625" customWidth="1"/>
+    <col min="3329" max="3329" width="39.83203125" customWidth="1"/>
+    <col min="3330" max="3330" width="23.1640625" customWidth="1"/>
+    <col min="3331" max="3331" width="16.83203125" customWidth="1"/>
+    <col min="3332" max="3332" width="17.5" customWidth="1"/>
+    <col min="3333" max="3333" width="17.1640625" customWidth="1"/>
+    <col min="3585" max="3585" width="39.83203125" customWidth="1"/>
+    <col min="3586" max="3586" width="23.1640625" customWidth="1"/>
+    <col min="3587" max="3587" width="16.83203125" customWidth="1"/>
+    <col min="3588" max="3588" width="17.5" customWidth="1"/>
+    <col min="3589" max="3589" width="17.1640625" customWidth="1"/>
+    <col min="3841" max="3841" width="39.83203125" customWidth="1"/>
+    <col min="3842" max="3842" width="23.1640625" customWidth="1"/>
+    <col min="3843" max="3843" width="16.83203125" customWidth="1"/>
+    <col min="3844" max="3844" width="17.5" customWidth="1"/>
+    <col min="3845" max="3845" width="17.1640625" customWidth="1"/>
+    <col min="4097" max="4097" width="39.83203125" customWidth="1"/>
+    <col min="4098" max="4098" width="23.1640625" customWidth="1"/>
+    <col min="4099" max="4099" width="16.83203125" customWidth="1"/>
+    <col min="4100" max="4100" width="17.5" customWidth="1"/>
+    <col min="4101" max="4101" width="17.1640625" customWidth="1"/>
+    <col min="4353" max="4353" width="39.83203125" customWidth="1"/>
+    <col min="4354" max="4354" width="23.1640625" customWidth="1"/>
+    <col min="4355" max="4355" width="16.83203125" customWidth="1"/>
+    <col min="4356" max="4356" width="17.5" customWidth="1"/>
+    <col min="4357" max="4357" width="17.1640625" customWidth="1"/>
+    <col min="4609" max="4609" width="39.83203125" customWidth="1"/>
+    <col min="4610" max="4610" width="23.1640625" customWidth="1"/>
+    <col min="4611" max="4611" width="16.83203125" customWidth="1"/>
+    <col min="4612" max="4612" width="17.5" customWidth="1"/>
+    <col min="4613" max="4613" width="17.1640625" customWidth="1"/>
+    <col min="4865" max="4865" width="39.83203125" customWidth="1"/>
+    <col min="4866" max="4866" width="23.1640625" customWidth="1"/>
+    <col min="4867" max="4867" width="16.83203125" customWidth="1"/>
+    <col min="4868" max="4868" width="17.5" customWidth="1"/>
+    <col min="4869" max="4869" width="17.1640625" customWidth="1"/>
+    <col min="5121" max="5121" width="39.83203125" customWidth="1"/>
+    <col min="5122" max="5122" width="23.1640625" customWidth="1"/>
+    <col min="5123" max="5123" width="16.83203125" customWidth="1"/>
+    <col min="5124" max="5124" width="17.5" customWidth="1"/>
+    <col min="5125" max="5125" width="17.1640625" customWidth="1"/>
+    <col min="5377" max="5377" width="39.83203125" customWidth="1"/>
+    <col min="5378" max="5378" width="23.1640625" customWidth="1"/>
+    <col min="5379" max="5379" width="16.83203125" customWidth="1"/>
+    <col min="5380" max="5380" width="17.5" customWidth="1"/>
+    <col min="5381" max="5381" width="17.1640625" customWidth="1"/>
+    <col min="5633" max="5633" width="39.83203125" customWidth="1"/>
+    <col min="5634" max="5634" width="23.1640625" customWidth="1"/>
+    <col min="5635" max="5635" width="16.83203125" customWidth="1"/>
+    <col min="5636" max="5636" width="17.5" customWidth="1"/>
+    <col min="5637" max="5637" width="17.1640625" customWidth="1"/>
+    <col min="5889" max="5889" width="39.83203125" customWidth="1"/>
+    <col min="5890" max="5890" width="23.1640625" customWidth="1"/>
+    <col min="5891" max="5891" width="16.83203125" customWidth="1"/>
+    <col min="5892" max="5892" width="17.5" customWidth="1"/>
+    <col min="5893" max="5893" width="17.1640625" customWidth="1"/>
+    <col min="6145" max="6145" width="39.83203125" customWidth="1"/>
+    <col min="6146" max="6146" width="23.1640625" customWidth="1"/>
+    <col min="6147" max="6147" width="16.83203125" customWidth="1"/>
+    <col min="6148" max="6148" width="17.5" customWidth="1"/>
+    <col min="6149" max="6149" width="17.1640625" customWidth="1"/>
+    <col min="6401" max="6401" width="39.83203125" customWidth="1"/>
+    <col min="6402" max="6402" width="23.1640625" customWidth="1"/>
+    <col min="6403" max="6403" width="16.83203125" customWidth="1"/>
+    <col min="6404" max="6404" width="17.5" customWidth="1"/>
+    <col min="6405" max="6405" width="17.1640625" customWidth="1"/>
+    <col min="6657" max="6657" width="39.83203125" customWidth="1"/>
+    <col min="6658" max="6658" width="23.1640625" customWidth="1"/>
+    <col min="6659" max="6659" width="16.83203125" customWidth="1"/>
+    <col min="6660" max="6660" width="17.5" customWidth="1"/>
+    <col min="6661" max="6661" width="17.1640625" customWidth="1"/>
+    <col min="6913" max="6913" width="39.83203125" customWidth="1"/>
+    <col min="6914" max="6914" width="23.1640625" customWidth="1"/>
+    <col min="6915" max="6915" width="16.83203125" customWidth="1"/>
+    <col min="6916" max="6916" width="17.5" customWidth="1"/>
+    <col min="6917" max="6917" width="17.1640625" customWidth="1"/>
+    <col min="7169" max="7169" width="39.83203125" customWidth="1"/>
+    <col min="7170" max="7170" width="23.1640625" customWidth="1"/>
+    <col min="7171" max="7171" width="16.83203125" customWidth="1"/>
+    <col min="7172" max="7172" width="17.5" customWidth="1"/>
+    <col min="7173" max="7173" width="17.1640625" customWidth="1"/>
+    <col min="7425" max="7425" width="39.83203125" customWidth="1"/>
+    <col min="7426" max="7426" width="23.1640625" customWidth="1"/>
+    <col min="7427" max="7427" width="16.83203125" customWidth="1"/>
+    <col min="7428" max="7428" width="17.5" customWidth="1"/>
+    <col min="7429" max="7429" width="17.1640625" customWidth="1"/>
+    <col min="7681" max="7681" width="39.83203125" customWidth="1"/>
+    <col min="7682" max="7682" width="23.1640625" customWidth="1"/>
+    <col min="7683" max="7683" width="16.83203125" customWidth="1"/>
+    <col min="7684" max="7684" width="17.5" customWidth="1"/>
+    <col min="7685" max="7685" width="17.1640625" customWidth="1"/>
+    <col min="7937" max="7937" width="39.83203125" customWidth="1"/>
+    <col min="7938" max="7938" width="23.1640625" customWidth="1"/>
+    <col min="7939" max="7939" width="16.83203125" customWidth="1"/>
+    <col min="7940" max="7940" width="17.5" customWidth="1"/>
+    <col min="7941" max="7941" width="17.1640625" customWidth="1"/>
+    <col min="8193" max="8193" width="39.83203125" customWidth="1"/>
+    <col min="8194" max="8194" width="23.1640625" customWidth="1"/>
+    <col min="8195" max="8195" width="16.83203125" customWidth="1"/>
+    <col min="8196" max="8196" width="17.5" customWidth="1"/>
+    <col min="8197" max="8197" width="17.1640625" customWidth="1"/>
+    <col min="8449" max="8449" width="39.83203125" customWidth="1"/>
+    <col min="8450" max="8450" width="23.1640625" customWidth="1"/>
+    <col min="8451" max="8451" width="16.83203125" customWidth="1"/>
+    <col min="8452" max="8452" width="17.5" customWidth="1"/>
+    <col min="8453" max="8453" width="17.1640625" customWidth="1"/>
+    <col min="8705" max="8705" width="39.83203125" customWidth="1"/>
+    <col min="8706" max="8706" width="23.1640625" customWidth="1"/>
+    <col min="8707" max="8707" width="16.83203125" customWidth="1"/>
+    <col min="8708" max="8708" width="17.5" customWidth="1"/>
+    <col min="8709" max="8709" width="17.1640625" customWidth="1"/>
+    <col min="8961" max="8961" width="39.83203125" customWidth="1"/>
+    <col min="8962" max="8962" width="23.1640625" customWidth="1"/>
+    <col min="8963" max="8963" width="16.83203125" customWidth="1"/>
+    <col min="8964" max="8964" width="17.5" customWidth="1"/>
+    <col min="8965" max="8965" width="17.1640625" customWidth="1"/>
+    <col min="9217" max="9217" width="39.83203125" customWidth="1"/>
+    <col min="9218" max="9218" width="23.1640625" customWidth="1"/>
+    <col min="9219" max="9219" width="16.83203125" customWidth="1"/>
+    <col min="9220" max="9220" width="17.5" customWidth="1"/>
+    <col min="9221" max="9221" width="17.1640625" customWidth="1"/>
+    <col min="9473" max="9473" width="39.83203125" customWidth="1"/>
+    <col min="9474" max="9474" width="23.1640625" customWidth="1"/>
+    <col min="9475" max="9475" width="16.83203125" customWidth="1"/>
+    <col min="9476" max="9476" width="17.5" customWidth="1"/>
+    <col min="9477" max="9477" width="17.1640625" customWidth="1"/>
+    <col min="9729" max="9729" width="39.83203125" customWidth="1"/>
+    <col min="9730" max="9730" width="23.1640625" customWidth="1"/>
+    <col min="9731" max="9731" width="16.83203125" customWidth="1"/>
+    <col min="9732" max="9732" width="17.5" customWidth="1"/>
+    <col min="9733" max="9733" width="17.1640625" customWidth="1"/>
+    <col min="9985" max="9985" width="39.83203125" customWidth="1"/>
+    <col min="9986" max="9986" width="23.1640625" customWidth="1"/>
+    <col min="9987" max="9987" width="16.83203125" customWidth="1"/>
+    <col min="9988" max="9988" width="17.5" customWidth="1"/>
+    <col min="9989" max="9989" width="17.1640625" customWidth="1"/>
+    <col min="10241" max="10241" width="39.83203125" customWidth="1"/>
+    <col min="10242" max="10242" width="23.1640625" customWidth="1"/>
+    <col min="10243" max="10243" width="16.83203125" customWidth="1"/>
+    <col min="10244" max="10244" width="17.5" customWidth="1"/>
+    <col min="10245" max="10245" width="17.1640625" customWidth="1"/>
+    <col min="10497" max="10497" width="39.83203125" customWidth="1"/>
+    <col min="10498" max="10498" width="23.1640625" customWidth="1"/>
+    <col min="10499" max="10499" width="16.83203125" customWidth="1"/>
+    <col min="10500" max="10500" width="17.5" customWidth="1"/>
+    <col min="10501" max="10501" width="17.1640625" customWidth="1"/>
+    <col min="10753" max="10753" width="39.83203125" customWidth="1"/>
+    <col min="10754" max="10754" width="23.1640625" customWidth="1"/>
+    <col min="10755" max="10755" width="16.83203125" customWidth="1"/>
+    <col min="10756" max="10756" width="17.5" customWidth="1"/>
+    <col min="10757" max="10757" width="17.1640625" customWidth="1"/>
+    <col min="11009" max="11009" width="39.83203125" customWidth="1"/>
+    <col min="11010" max="11010" width="23.1640625" customWidth="1"/>
+    <col min="11011" max="11011" width="16.83203125" customWidth="1"/>
+    <col min="11012" max="11012" width="17.5" customWidth="1"/>
+    <col min="11013" max="11013" width="17.1640625" customWidth="1"/>
+    <col min="11265" max="11265" width="39.83203125" customWidth="1"/>
+    <col min="11266" max="11266" width="23.1640625" customWidth="1"/>
+    <col min="11267" max="11267" width="16.83203125" customWidth="1"/>
+    <col min="11268" max="11268" width="17.5" customWidth="1"/>
+    <col min="11269" max="11269" width="17.1640625" customWidth="1"/>
+    <col min="11521" max="11521" width="39.83203125" customWidth="1"/>
+    <col min="11522" max="11522" width="23.1640625" customWidth="1"/>
+    <col min="11523" max="11523" width="16.83203125" customWidth="1"/>
+    <col min="11524" max="11524" width="17.5" customWidth="1"/>
+    <col min="11525" max="11525" width="17.1640625" customWidth="1"/>
+    <col min="11777" max="11777" width="39.83203125" customWidth="1"/>
+    <col min="11778" max="11778" width="23.1640625" customWidth="1"/>
+    <col min="11779" max="11779" width="16.83203125" customWidth="1"/>
+    <col min="11780" max="11780" width="17.5" customWidth="1"/>
+    <col min="11781" max="11781" width="17.1640625" customWidth="1"/>
+    <col min="12033" max="12033" width="39.83203125" customWidth="1"/>
+    <col min="12034" max="12034" width="23.1640625" customWidth="1"/>
+    <col min="12035" max="12035" width="16.83203125" customWidth="1"/>
+    <col min="12036" max="12036" width="17.5" customWidth="1"/>
+    <col min="12037" max="12037" width="17.1640625" customWidth="1"/>
+    <col min="12289" max="12289" width="39.83203125" customWidth="1"/>
+    <col min="12290" max="12290" width="23.1640625" customWidth="1"/>
+    <col min="12291" max="12291" width="16.83203125" customWidth="1"/>
+    <col min="12292" max="12292" width="17.5" customWidth="1"/>
+    <col min="12293" max="12293" width="17.1640625" customWidth="1"/>
+    <col min="12545" max="12545" width="39.83203125" customWidth="1"/>
+    <col min="12546" max="12546" width="23.1640625" customWidth="1"/>
+    <col min="12547" max="12547" width="16.83203125" customWidth="1"/>
+    <col min="12548" max="12548" width="17.5" customWidth="1"/>
+    <col min="12549" max="12549" width="17.1640625" customWidth="1"/>
+    <col min="12801" max="12801" width="39.83203125" customWidth="1"/>
+    <col min="12802" max="12802" width="23.1640625" customWidth="1"/>
+    <col min="12803" max="12803" width="16.83203125" customWidth="1"/>
+    <col min="12804" max="12804" width="17.5" customWidth="1"/>
+    <col min="12805" max="12805" width="17.1640625" customWidth="1"/>
+    <col min="13057" max="13057" width="39.83203125" customWidth="1"/>
+    <col min="13058" max="13058" width="23.1640625" customWidth="1"/>
+    <col min="13059" max="13059" width="16.83203125" customWidth="1"/>
+    <col min="13060" max="13060" width="17.5" customWidth="1"/>
+    <col min="13061" max="13061" width="17.1640625" customWidth="1"/>
+    <col min="13313" max="13313" width="39.83203125" customWidth="1"/>
+    <col min="13314" max="13314" width="23.1640625" customWidth="1"/>
+    <col min="13315" max="13315" width="16.83203125" customWidth="1"/>
+    <col min="13316" max="13316" width="17.5" customWidth="1"/>
+    <col min="13317" max="13317" width="17.1640625" customWidth="1"/>
+    <col min="13569" max="13569" width="39.83203125" customWidth="1"/>
+    <col min="13570" max="13570" width="23.1640625" customWidth="1"/>
+    <col min="13571" max="13571" width="16.83203125" customWidth="1"/>
+    <col min="13572" max="13572" width="17.5" customWidth="1"/>
+    <col min="13573" max="13573" width="17.1640625" customWidth="1"/>
+    <col min="13825" max="13825" width="39.83203125" customWidth="1"/>
+    <col min="13826" max="13826" width="23.1640625" customWidth="1"/>
+    <col min="13827" max="13827" width="16.83203125" customWidth="1"/>
+    <col min="13828" max="13828" width="17.5" customWidth="1"/>
+    <col min="13829" max="13829" width="17.1640625" customWidth="1"/>
+    <col min="14081" max="14081" width="39.83203125" customWidth="1"/>
+    <col min="14082" max="14082" width="23.1640625" customWidth="1"/>
+    <col min="14083" max="14083" width="16.83203125" customWidth="1"/>
+    <col min="14084" max="14084" width="17.5" customWidth="1"/>
+    <col min="14085" max="14085" width="17.1640625" customWidth="1"/>
+    <col min="14337" max="14337" width="39.83203125" customWidth="1"/>
+    <col min="14338" max="14338" width="23.1640625" customWidth="1"/>
+    <col min="14339" max="14339" width="16.83203125" customWidth="1"/>
+    <col min="14340" max="14340" width="17.5" customWidth="1"/>
+    <col min="14341" max="14341" width="17.1640625" customWidth="1"/>
+    <col min="14593" max="14593" width="39.83203125" customWidth="1"/>
+    <col min="14594" max="14594" width="23.1640625" customWidth="1"/>
+    <col min="14595" max="14595" width="16.83203125" customWidth="1"/>
+    <col min="14596" max="14596" width="17.5" customWidth="1"/>
+    <col min="14597" max="14597" width="17.1640625" customWidth="1"/>
+    <col min="14849" max="14849" width="39.83203125" customWidth="1"/>
+    <col min="14850" max="14850" width="23.1640625" customWidth="1"/>
+    <col min="14851" max="14851" width="16.83203125" customWidth="1"/>
+    <col min="14852" max="14852" width="17.5" customWidth="1"/>
+    <col min="14853" max="14853" width="17.1640625" customWidth="1"/>
+    <col min="15105" max="15105" width="39.83203125" customWidth="1"/>
+    <col min="15106" max="15106" width="23.1640625" customWidth="1"/>
+    <col min="15107" max="15107" width="16.83203125" customWidth="1"/>
+    <col min="15108" max="15108" width="17.5" customWidth="1"/>
+    <col min="15109" max="15109" width="17.1640625" customWidth="1"/>
+    <col min="15361" max="15361" width="39.83203125" customWidth="1"/>
+    <col min="15362" max="15362" width="23.1640625" customWidth="1"/>
+    <col min="15363" max="15363" width="16.83203125" customWidth="1"/>
+    <col min="15364" max="15364" width="17.5" customWidth="1"/>
+    <col min="15365" max="15365" width="17.1640625" customWidth="1"/>
+    <col min="15617" max="15617" width="39.83203125" customWidth="1"/>
+    <col min="15618" max="15618" width="23.1640625" customWidth="1"/>
+    <col min="15619" max="15619" width="16.83203125" customWidth="1"/>
+    <col min="15620" max="15620" width="17.5" customWidth="1"/>
+    <col min="15621" max="15621" width="17.1640625" customWidth="1"/>
+    <col min="15873" max="15873" width="39.83203125" customWidth="1"/>
+    <col min="15874" max="15874" width="23.1640625" customWidth="1"/>
+    <col min="15875" max="15875" width="16.83203125" customWidth="1"/>
+    <col min="15876" max="15876" width="17.5" customWidth="1"/>
+    <col min="15877" max="15877" width="17.1640625" customWidth="1"/>
+    <col min="16129" max="16129" width="39.83203125" customWidth="1"/>
+    <col min="16130" max="16130" width="23.1640625" customWidth="1"/>
+    <col min="16131" max="16131" width="16.83203125" customWidth="1"/>
+    <col min="16132" max="16132" width="17.5" customWidth="1"/>
+    <col min="16133" max="16133" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="6" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="26" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="24" t="s">
         <v>168</v>
       </c>
-      <c r="B2" s="19"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="26"/>
-      <c r="B3" s="19"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B2" s="17"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="24"/>
+      <c r="B3" s="17"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B7" s="18"/>
-      <c r="E7" s="27" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B7" s="14"/>
+      <c r="E7" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="64">
+      <c r="C8" s="51">
         <v>12</v>
       </c>
       <c r="E8" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B9" s="18" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B9" s="14" t="s">
         <v>29</v>
       </c>
       <c r="C9">
@@ -3263,117 +3242,114 @@
         <v>8.3333333333333338E-8</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="18"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B10" s="14"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="64">
+      <c r="C11" s="51">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="38"/>
-      <c r="B12" s="109"/>
-      <c r="C12" s="95"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B13" s="18"/>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="4"/>
+      <c r="B12" s="14"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B13" s="14"/>
       <c r="C13" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="D13" s="38"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D13" s="4"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="95">
+      <c r="C14">
         <f>1.41*C15</f>
         <v>1.41</v>
       </c>
-      <c r="D14" s="34"/>
       <c r="E14" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B15" s="18" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B15" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="C15" s="88">
+      <c r="C15" s="75">
         <v>1</v>
       </c>
-      <c r="D15" s="28"/>
+      <c r="D15" s="3"/>
       <c r="E15" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="14" t="s">
         <v>163</v>
       </c>
-      <c r="C16" s="64">
+      <c r="C16" s="51">
         <v>4.5</v>
       </c>
-      <c r="D16" s="28"/>
+      <c r="D16" s="3"/>
       <c r="E16" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B17" s="18"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B17" s="14"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="64">
+      <c r="C18" s="51">
         <v>3</v>
       </c>
-      <c r="D18" s="34"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B19" s="18" t="s">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B19" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="77">
+      <c r="C19" s="64">
         <f>(24+32*C18)*C9</f>
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="D19" s="34" t="s">
+      <c r="D19" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B20" s="18" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B20" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="20">
+      <c r="C20" s="18">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B21" s="18" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B21" s="14" t="s">
         <v>231</v>
       </c>
-      <c r="C21" s="21">
+      <c r="C21" s="19">
         <f>C9*(16+8*C20)</f>
         <v>2.6666666666666668E-6</v>
       </c>
@@ -3381,186 +3357,186 @@
         <v>232</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="29" t="s">
+    <row r="22" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A22" s="26" t="s">
         <v>184</v>
       </c>
-      <c r="B22" s="91" t="s">
+      <c r="B22" s="78" t="s">
         <v>65</v>
       </c>
-      <c r="C22" s="92">
+      <c r="C22" s="79">
         <f>1/((2+4*C23)*C19)/1000</f>
         <v>28.571428571428569</v>
       </c>
-      <c r="D22" s="28"/>
+      <c r="D22" s="3"/>
       <c r="E22" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A23" s="29" t="s">
+    <row r="23" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A23" s="26" t="s">
         <v>164</v>
       </c>
-      <c r="B23" s="37" t="s">
+      <c r="B23" s="30" t="s">
         <v>166</v>
       </c>
-      <c r="C23" s="96">
+      <c r="C23" s="44">
         <f>MIN(MAX(0.2,2*(C16*C15)/$C11),0.9)</f>
         <v>0.375</v>
       </c>
-      <c r="D23" s="28"/>
+      <c r="D23" s="3"/>
       <c r="E23" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B24" s="18"/>
-      <c r="C24" s="28"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B25" s="18"/>
-      <c r="C25" s="40" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B24" s="14"/>
+      <c r="C24" s="3"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B25" s="14"/>
+      <c r="C25" s="31" t="s">
         <v>127</v>
       </c>
-      <c r="D25" s="38"/>
-      <c r="E25" s="38"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="B26" s="18"/>
+      <c r="B26" s="14"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>68</v>
       </c>
-      <c r="B27" s="18" t="s">
+      <c r="B27" s="14" t="s">
         <v>69</v>
       </c>
       <c r="C27">
         <v>0.17</v>
       </c>
-      <c r="E27" s="30"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="24" t="s">
+      <c r="E27" s="9"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="B28" s="18" t="s">
+      <c r="B28" s="14" t="s">
         <v>71</v>
       </c>
       <c r="C28">
         <v>0.17</v>
       </c>
-      <c r="E28" s="30"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B29" s="18"/>
-      <c r="E29" s="30"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E28" s="9"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B29" s="14"/>
+      <c r="E29" s="9"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>155</v>
       </c>
-      <c r="B30" s="18" t="s">
+      <c r="B30" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="C30" s="89">
+      <c r="C30" s="76">
         <v>70</v>
       </c>
-      <c r="D30" s="31"/>
+      <c r="D30" s="23"/>
       <c r="E30" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B31" s="18" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B31" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="C31" s="22">
+      <c r="C31" s="20">
         <f>C27*(1+(0.55*(C30-25)/100))</f>
         <v>0.21207500000000001</v>
       </c>
       <c r="D31" s="3"/>
-      <c r="E31" s="22"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B32" s="18" t="s">
+      <c r="E31" s="20"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B32" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="C32" s="22">
+      <c r="C32" s="20">
         <f>C28*(1+(0.55*(C30-25)/100))</f>
         <v>0.21207500000000001</v>
       </c>
       <c r="D32" s="3"/>
-      <c r="E32" s="22"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B33" s="15"/>
+      <c r="E32" s="20"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B33" s="14"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
-      <c r="E33" s="22"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E33" s="20"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>74</v>
       </c>
-      <c r="B34" s="18" t="s">
+      <c r="B34" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="C34" s="25">
+      <c r="C34" s="23">
         <v>30</v>
       </c>
-      <c r="D34" s="25"/>
+      <c r="D34" s="23"/>
       <c r="E34" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B35" s="18" t="s">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B35" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="C35" s="25">
+      <c r="C35" s="23">
         <v>40</v>
       </c>
-      <c r="D35" s="25"/>
-      <c r="E35" s="31"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B36" s="18" t="s">
+      <c r="D35" s="23"/>
+      <c r="E35" s="23"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B36" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="C36" s="25">
+      <c r="C36" s="23">
         <v>60</v>
       </c>
-      <c r="D36" s="25"/>
-      <c r="E36" s="25"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B37" s="18" t="s">
+      <c r="D36" s="23"/>
+      <c r="E36" s="23"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B37" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="C37" s="25">
+      <c r="C37" s="23">
         <v>60</v>
       </c>
-      <c r="D37" s="25"/>
-      <c r="E37" s="25"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B38" s="18"/>
-      <c r="C38" s="25"/>
-      <c r="D38" s="25"/>
-      <c r="E38" s="25"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="47" t="s">
+      <c r="D37" s="23"/>
+      <c r="E37" s="23"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B38" s="14"/>
+      <c r="C38" s="23"/>
+      <c r="D38" s="23"/>
+      <c r="E38" s="23"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>80</v>
       </c>
-      <c r="B39" s="18" t="s">
+      <c r="B39" s="14" t="s">
         <v>81</v>
       </c>
       <c r="C39" s="3">
@@ -3570,37 +3546,37 @@
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="13" t="s">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>82</v>
       </c>
-      <c r="B40" s="18" t="s">
+      <c r="B40" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="C40" s="22">
+      <c r="C40" s="20">
         <f>$C$22*1000*((C36+C35)/1000000000)*$C$11*$C$15*2/2</f>
         <v>6.8571428571428561E-2</v>
       </c>
-      <c r="D40" s="22"/>
-      <c r="E40" s="22"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="34" t="s">
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>84</v>
       </c>
-      <c r="B41" s="15" t="s">
+      <c r="B41" s="14" t="s">
         <v>85</v>
       </c>
       <c r="C41" s="8">
         <f>C39+C40</f>
         <v>0.14809955357142857</v>
       </c>
-      <c r="D41" s="39"/>
-      <c r="E41" s="39"/>
-      <c r="G41" s="32"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B42" s="18" t="s">
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="G41" s="27"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B42" s="14" t="s">
         <v>86</v>
       </c>
       <c r="C42" s="3">
@@ -3610,144 +3586,143 @@
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B43" s="18" t="s">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B43" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="C43" s="22">
+      <c r="C43" s="20">
         <f>C22*1000*((C37+C34)/1000000000)*$C$11*C15*2/2</f>
         <v>6.1714285714285708E-2</v>
       </c>
-      <c r="D43" s="22"/>
-      <c r="E43" s="22"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="34" t="s">
+      <c r="D43" s="20"/>
+      <c r="E43" s="20"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>84</v>
       </c>
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="14" t="s">
         <v>88</v>
       </c>
       <c r="C44" s="8">
         <f>C42+C43</f>
         <v>0.19426116071428573</v>
       </c>
-      <c r="D44" s="39"/>
-      <c r="E44" s="39"/>
-      <c r="G44" s="32"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" s="13"/>
-      <c r="B45" s="15"/>
-      <c r="C45" s="39"/>
-      <c r="D45" s="39"/>
-      <c r="E45" s="39"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="G44" s="27"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B45" s="14"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>89</v>
       </c>
-      <c r="B46" s="15" t="s">
+      <c r="B46" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="C46" s="39">
+      <c r="C46" s="3">
         <f>2*C42+C43+2*C39+C40</f>
         <v>0.55443571428571436</v>
       </c>
-      <c r="D46" s="39"/>
-      <c r="E46" s="39"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="38" t="s">
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="B47" s="15" t="s">
+      <c r="B47" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="C47" s="39">
+      <c r="C47" s="3">
         <f>2*C46</f>
         <v>1.1088714285714287</v>
       </c>
-      <c r="D47" s="39"/>
-      <c r="E47" s="39"/>
-      <c r="G47" s="32"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" s="38" t="s">
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="G47" s="27"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="B48" s="18" t="s">
+      <c r="B48" s="14" t="s">
         <v>176</v>
       </c>
-      <c r="C48" s="39">
+      <c r="C48" s="3">
         <f>C11*(0.0025+0.0005+C8*0.0003)</f>
         <v>0.15839999999999999</v>
       </c>
-      <c r="D48" s="39"/>
-      <c r="E48" s="39"/>
-      <c r="G48" s="32"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" s="38"/>
-      <c r="B49" s="14"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="G48" s="27"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" s="4"/>
+      <c r="B49" s="13"/>
       <c r="C49" s="8"/>
       <c r="D49" s="8"/>
       <c r="E49" s="8"/>
-      <c r="G49" s="32"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A50" s="38" t="s">
+      <c r="G49" s="27"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="B50" s="14" t="s">
+      <c r="B50" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="C50" s="40">
+      <c r="C50" s="31">
         <f>C47+C48</f>
         <v>1.2672714285714286</v>
       </c>
-      <c r="E50" s="48"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A51" s="38"/>
-      <c r="B51" s="14"/>
+      <c r="E50" s="8"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51" s="4"/>
+      <c r="B51" s="13"/>
       <c r="C51" s="8"/>
       <c r="E51" s="8"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A53" s="38" t="s">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="B53" s="18" t="s">
+      <c r="B53" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="C53" s="90">
+      <c r="C53" s="77">
         <v>0.1</v>
       </c>
-      <c r="D53" s="49"/>
+      <c r="D53" s="37"/>
       <c r="E53" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B54" s="93" t="s">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B54" s="80" t="s">
         <v>159</v>
       </c>
-      <c r="C54" s="94">
+      <c r="C54" s="81">
         <f>C$53*C$15^2*C$23</f>
         <v>3.7500000000000006E-2</v>
       </c>
-      <c r="D54" s="48"/>
+      <c r="D54" s="8"/>
       <c r="E54" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="G54" s="32"/>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B55" s="93" t="s">
+      <c r="G54" s="27"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B55" s="80" t="s">
         <v>160</v>
       </c>
-      <c r="C55" s="94">
+      <c r="C55" s="81">
         <f>C$53*C$15^2*0.7</f>
         <v>6.9999999999999993E-2</v>
       </c>
@@ -3755,43 +3730,43 @@
         <v>161</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="12"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="12"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="12"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="12"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="12"/>
       <c r="B63" s="3"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="12"/>
       <c r="B64" s="3"/>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="12"/>
-      <c r="B65" s="33"/>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B65" s="28"/>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="12"/>
       <c r="B66" s="3"/>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="12"/>
       <c r="B67" s="3"/>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="12"/>
       <c r="B68" s="3"/>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="12"/>
       <c r="B69" s="3"/>
     </row>
@@ -3809,15 +3784,15 @@
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.6640625" customWidth="1"/>
-    <col min="2" max="2" width="17.44140625" customWidth="1"/>
-    <col min="3" max="3" width="16.109375" customWidth="1"/>
-    <col min="4" max="4" width="39.88671875" customWidth="1"/>
+    <col min="2" max="2" width="17.5" customWidth="1"/>
+    <col min="3" max="3" width="16.1640625" customWidth="1"/>
+    <col min="4" max="4" width="39.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>137</v>
       </c>
@@ -3828,7 +3803,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>138</v>
       </c>
@@ -3839,12 +3814,12 @@
         <v>139</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>142</v>
       </c>
@@ -3862,7 +3837,7 @@
       </c>
       <c r="F5"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -3879,7 +3854,7 @@
         <v>5.0761726259131092E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>0.82</v>
       </c>
@@ -3896,7 +3871,7 @@
         <v>6.1375070861677997E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>0.75</v>
       </c>
@@ -3913,7 +3888,7 @@
         <v>6.6806164614606187E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>0.68</v>
       </c>
@@ -3933,7 +3908,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>0.5</v>
       </c>
@@ -3950,7 +3925,7 @@
         <v>9.7656249999999986E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>0.47</v>
       </c>
@@ -3967,7 +3942,7 @@
         <v>0.10338140358184091</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>0.33</v>
       </c>
@@ -3984,7 +3959,7 @@
         <v>0.14227040816326525</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>0.27</v>
       </c>
@@ -4001,7 +3976,7 @@
         <v>0.16955261593341256</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>0.22</v>
       </c>
@@ -4021,7 +3996,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>0.15</v>
       </c>
@@ -4038,15 +4013,15 @@
         <v>0.27411332179930797</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>0.12</v>
       </c>
-      <c r="B16" s="56">
+      <c r="B16" s="44">
         <f t="shared" si="0"/>
         <v>2.3214285714285716</v>
       </c>
-      <c r="C16" s="56">
+      <c r="C16" s="44">
         <f t="shared" si="1"/>
         <v>1.6414978848973425</v>
       </c>
@@ -4055,15 +4030,15 @@
         <v>0.32334183673469391</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>0.1</v>
       </c>
-      <c r="B17" s="56">
+      <c r="B17" s="44">
         <f t="shared" si="0"/>
         <v>2.708333333333333</v>
       </c>
-      <c r="C17" s="56">
+      <c r="C17" s="44">
         <f t="shared" si="1"/>
         <v>1.9150808657135658</v>
       </c>
@@ -4072,15 +4047,15 @@
         <v>0.3667534722222221</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="B18" s="55">
+      <c r="B18" s="43">
         <f t="shared" ref="B18" si="3">$B$1/(A18+0.02)/1000</f>
         <v>3.4210526315789473</v>
       </c>
-      <c r="C18" s="55">
+      <c r="C18" s="43">
         <f t="shared" ref="C18" si="4">B18/SQRT(2)</f>
         <v>2.4190495145855571</v>
       </c>
@@ -4092,19 +4067,19 @@
         <v>147</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D20" s="3"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>144</v>
       </c>
       <c r="D21" s="3"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>142</v>
       </c>
@@ -4119,7 +4094,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1</v>
       </c>
@@ -4136,7 +4111,7 @@
         <v>1.5570934256055362E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>0.82</v>
       </c>
@@ -4153,7 +4128,7 @@
         <v>1.8826530612244898E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>0.75</v>
       </c>
@@ -4170,7 +4145,7 @@
         <v>2.0492494518468539E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>0.68</v>
       </c>
@@ -4187,7 +4162,7 @@
         <v>2.2481632653061218E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>0.5</v>
       </c>
@@ -4204,7 +4179,7 @@
         <v>2.9955621301775138E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>0.47</v>
       </c>
@@ -4221,7 +4196,7 @@
         <v>3.1711786755518535E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>0.33</v>
       </c>
@@ -4238,7 +4213,7 @@
         <v>4.36408163265306E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>0.27</v>
       </c>
@@ -4255,7 +4230,7 @@
         <v>5.200951248513673E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>0.22</v>
       </c>
@@ -4272,7 +4247,7 @@
         <v>6.1874999999999986E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>0.15</v>
       </c>
@@ -4292,7 +4267,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>0.12</v>
       </c>
@@ -4309,15 +4284,15 @@
         <v>9.9183673469387751E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>0.1</v>
       </c>
-      <c r="B34" s="56">
+      <c r="B34" s="44">
         <f t="shared" si="6"/>
         <v>1.4999999999999998</v>
       </c>
-      <c r="C34" s="56">
+      <c r="C34" s="44">
         <f t="shared" si="7"/>
         <v>1.060660171779821</v>
       </c>
@@ -4326,7 +4301,7 @@
         <v>0.11249999999999993</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>8.2000000000000003E-2</v>
       </c>
@@ -4343,7 +4318,7 @@
         <v>0.12768166089965391</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -4360,15 +4335,15 @@
         <v>0.13462603878116342</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>6.8000000000000005E-2</v>
       </c>
-      <c r="B37" s="56">
+      <c r="B37" s="44">
         <f t="shared" si="6"/>
         <v>2.0454545454545454</v>
       </c>
-      <c r="C37" s="56">
+      <c r="C37" s="44">
         <f t="shared" si="7"/>
         <v>1.4463547796997562</v>
       </c>
@@ -4380,15 +4355,15 @@
         <v>146</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>4.7E-2</v>
       </c>
-      <c r="B38" s="55">
+      <c r="B38" s="43">
         <f t="shared" ref="B38" si="9">$B$2/(A38+0.02)/1000</f>
         <v>2.6865671641791042</v>
       </c>
-      <c r="C38" s="55">
+      <c r="C38" s="43">
         <f t="shared" ref="C38" si="10">B38/SQRT(2)</f>
         <v>1.8996898599041572</v>
       </c>
@@ -4396,19 +4371,19 @@
         <f t="shared" ref="D38" si="11">A38*C38*C38</f>
         <v>0.16961461349966581</v>
       </c>
-      <c r="F38" s="32" t="s">
+      <c r="F38" s="27" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="B39" s="55">
+      <c r="B39" s="43">
         <f t="shared" ref="B39" si="12">$B$2/(A39+0.02)/1000</f>
         <v>3.3962264150943393</v>
       </c>
-      <c r="C39" s="55">
+      <c r="C39" s="43">
         <f t="shared" ref="C39" si="13">B39/SQRT(2)</f>
         <v>2.4014947285580854</v>
       </c>
@@ -4416,18 +4391,18 @@
         <f t="shared" ref="D39" si="14">A39*C39*C39</f>
         <v>0.19031683873264502</v>
       </c>
-      <c r="F39" s="32" t="s">
+      <c r="F39" s="27" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D40" s="3"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D41" s="3"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C42" s="24" t="s">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C42" s="22" t="s">
         <v>189</v>
       </c>
     </row>
@@ -4445,63 +4420,63 @@
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.109375" customWidth="1"/>
-    <col min="2" max="2" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.44140625" customWidth="1"/>
-    <col min="5" max="5" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.109375" customWidth="1"/>
+    <col min="1" max="1" width="14.1640625" customWidth="1"/>
+    <col min="2" max="2" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5" customWidth="1"/>
+    <col min="5" max="5" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" s="6" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" s="6" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="51" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="39" t="s">
         <v>133</v>
       </c>
-      <c r="B4" s="53" t="s">
+      <c r="B4" s="41" t="s">
         <v>129</v>
       </c>
-      <c r="C4" s="50" t="s">
+      <c r="C4" s="38" t="s">
         <v>134</v>
       </c>
-      <c r="D4" s="50" t="s">
+      <c r="D4" s="38" t="s">
         <v>182</v>
       </c>
-      <c r="E4" s="50" t="s">
+      <c r="E4" s="38" t="s">
         <v>135</v>
       </c>
-      <c r="F4" s="50" t="s">
+      <c r="F4" s="38" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="52">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="40">
         <v>6.2</v>
       </c>
-      <c r="B5" s="54">
+      <c r="B5" s="42">
         <f>5/(0.4+A5)/1000+2.5/67000</f>
         <v>7.9488919041157844E-4</v>
       </c>
-      <c r="C5" s="99">
+      <c r="C5" s="84">
         <f>B5*$B$20</f>
         <v>2.6231343283582089</v>
       </c>
-      <c r="D5" s="100">
+      <c r="D5" s="85">
         <f>C5/SQRT(2)</f>
         <v>1.8548360715453092</v>
       </c>
-      <c r="E5" s="97">
+      <c r="E5" s="82">
         <f>0.55*C5</f>
         <v>1.4427238805970151</v>
       </c>
@@ -4510,23 +4485,23 @@
         <v>1.0201598393499203</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="52">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="40">
         <v>6.8</v>
       </c>
-      <c r="B6" s="54">
+      <c r="B6" s="42">
         <f>5/(0.4+A6)/1000+2.5/67000</f>
         <v>7.3175787728026534E-4</v>
       </c>
-      <c r="C6" s="111">
+      <c r="C6" s="95">
         <f t="shared" ref="C6:C18" si="0">B6*$B$20</f>
         <v>2.4148009950248754</v>
       </c>
-      <c r="D6" s="98">
+      <c r="D6" s="83">
         <f t="shared" ref="D6:D18" si="1">C6/SQRT(2)</f>
         <v>1.7075221587981118</v>
       </c>
-      <c r="E6" s="98">
+      <c r="E6" s="83">
         <f>0.55*C6</f>
         <v>1.3281405472636816</v>
       </c>
@@ -4535,23 +4510,23 @@
         <v>0.93913718733896145</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="52">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="40">
         <v>7.5</v>
       </c>
-      <c r="B7" s="54">
+      <c r="B7" s="42">
         <f t="shared" ref="B7:B18" si="3">5/(0.4+A7)/1000+2.5/67000</f>
         <v>6.7022482524088406E-4</v>
       </c>
-      <c r="C7" s="110">
+      <c r="C7" s="94">
         <f t="shared" si="0"/>
         <v>2.2117419232949174</v>
       </c>
-      <c r="D7" s="98">
+      <c r="D7" s="83">
         <f t="shared" si="1"/>
         <v>1.5639377121964129</v>
       </c>
-      <c r="E7" s="98">
+      <c r="E7" s="83">
         <f t="shared" ref="E7:E18" si="4">0.55*C7</f>
         <v>1.2164580578122046</v>
       </c>
@@ -4560,23 +4535,23 @@
         <v>0.86016574170802707</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="52">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="40">
         <v>8.1999999999999993</v>
       </c>
-      <c r="B8" s="54">
+      <c r="B8" s="42">
         <f t="shared" si="3"/>
         <v>6.1870878167303016E-4</v>
       </c>
-      <c r="C8" s="110">
+      <c r="C8" s="94">
         <f t="shared" si="0"/>
         <v>2.0417389795209995</v>
       </c>
-      <c r="D8" s="98">
+      <c r="D8" s="83">
         <f t="shared" si="1"/>
         <v>1.4437274778322</v>
       </c>
-      <c r="E8" s="98">
+      <c r="E8" s="83">
         <f t="shared" si="4"/>
         <v>1.1229564387365498</v>
       </c>
@@ -4585,23 +4560,23 @@
         <v>0.7940501128077101</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="52">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="40">
         <v>9.1</v>
       </c>
-      <c r="B9" s="54">
+      <c r="B9" s="42">
         <f t="shared" si="3"/>
         <v>5.6362922230950507E-4</v>
       </c>
-      <c r="C9" s="110">
+      <c r="C9" s="94">
         <f t="shared" si="0"/>
         <v>1.8599764336213667</v>
       </c>
-      <c r="D9" s="98">
+      <c r="D9" s="83">
         <f t="shared" si="1"/>
         <v>1.3152019490608386</v>
       </c>
-      <c r="E9" s="98">
+      <c r="E9" s="83">
         <f t="shared" si="4"/>
         <v>1.0229870384917517</v>
       </c>
@@ -4610,23 +4585,23 @@
         <v>0.72336107198346122</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="52">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="40">
         <v>10</v>
       </c>
-      <c r="B10" s="54">
+      <c r="B10" s="42">
         <f t="shared" si="3"/>
         <v>5.1808266360505166E-4</v>
       </c>
-      <c r="C10" s="110">
+      <c r="C10" s="94">
         <f t="shared" si="0"/>
         <v>1.7096727898966706</v>
       </c>
-      <c r="D10" s="98">
+      <c r="D10" s="83">
         <f t="shared" si="1"/>
         <v>1.2089212233460591</v>
       </c>
-      <c r="E10" s="98">
+      <c r="E10" s="83">
         <f t="shared" si="4"/>
         <v>0.94032003444316892</v>
       </c>
@@ -4635,23 +4610,23 @@
         <v>0.66490667284033267</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="52">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="40">
         <v>12</v>
       </c>
-      <c r="B11" s="54">
+      <c r="B11" s="42">
         <f t="shared" si="3"/>
         <v>4.4053923928743383E-4</v>
       </c>
-      <c r="C11" s="110">
+      <c r="C11" s="94">
         <f t="shared" si="0"/>
         <v>1.4537794896485317</v>
       </c>
-      <c r="D11" s="98">
+      <c r="D11" s="83">
         <f t="shared" si="1"/>
         <v>1.0279773354803949</v>
       </c>
-      <c r="E11" s="98">
+      <c r="E11" s="83">
         <f t="shared" si="4"/>
         <v>0.79957871930669244</v>
       </c>
@@ -4660,23 +4635,23 @@
         <v>0.56538753451421719</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="52">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="40">
         <v>15</v>
       </c>
-      <c r="B12" s="54">
+      <c r="B12" s="42">
         <f t="shared" si="3"/>
         <v>3.6198875751114554E-4</v>
       </c>
-      <c r="C12" s="110">
+      <c r="C12" s="94">
         <f t="shared" si="0"/>
         <v>1.1945628997867803</v>
       </c>
-      <c r="D12" s="98">
+      <c r="D12" s="83">
         <f t="shared" si="1"/>
         <v>0.84468352699309857</v>
       </c>
-      <c r="E12" s="98">
+      <c r="E12" s="83">
         <f t="shared" si="4"/>
         <v>0.65700959488272925</v>
       </c>
@@ -4685,23 +4660,23 @@
         <v>0.46457593984620421</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="52">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="40">
         <v>18</v>
       </c>
-      <c r="B13" s="54">
+      <c r="B13" s="42">
         <f t="shared" si="3"/>
         <v>3.0905256327060353E-4</v>
       </c>
-      <c r="C13" s="110">
+      <c r="C13" s="94">
         <f t="shared" si="0"/>
         <v>1.0198734587929916</v>
       </c>
-      <c r="D13" s="98">
+      <c r="D13" s="83">
         <f t="shared" si="1"/>
         <v>0.72115943866470322</v>
       </c>
-      <c r="E13" s="98">
+      <c r="E13" s="83">
         <f t="shared" si="4"/>
         <v>0.56093040233614544</v>
       </c>
@@ -4710,23 +4685,23 @@
         <v>0.39663769126558684</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="52">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="40">
         <v>22</v>
       </c>
-      <c r="B14" s="54">
+      <c r="B14" s="42">
         <f t="shared" si="3"/>
         <v>2.6052771855010666E-4</v>
       </c>
-      <c r="C14" s="110">
+      <c r="C14" s="94">
         <f t="shared" si="0"/>
         <v>0.85974147121535194</v>
       </c>
-      <c r="D14" s="98">
+      <c r="D14" s="83">
         <f t="shared" si="1"/>
         <v>0.60792902436367424</v>
       </c>
-      <c r="E14" s="98">
+      <c r="E14" s="83">
         <f t="shared" si="4"/>
         <v>0.47285780916844361</v>
       </c>
@@ -4735,23 +4710,23 @@
         <v>0.33436096340002086</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="52">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="40">
         <v>24</v>
       </c>
-      <c r="B15" s="54">
+      <c r="B15" s="42">
         <f t="shared" si="3"/>
         <v>2.4223146562270614E-4</v>
       </c>
-      <c r="C15" s="110">
+      <c r="C15" s="94">
         <f t="shared" si="0"/>
         <v>0.79936383655493026</v>
       </c>
-      <c r="D15" s="98">
+      <c r="D15" s="83">
         <f t="shared" si="1"/>
         <v>0.56523558946328623</v>
       </c>
-      <c r="E15" s="98">
+      <c r="E15" s="83">
         <f t="shared" si="4"/>
         <v>0.43965011010521166</v>
       </c>
@@ -4760,23 +4735,23 @@
         <v>0.31087957420480739</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="52">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="40">
         <v>27</v>
       </c>
-      <c r="B16" s="54">
+      <c r="B16" s="42">
         <f t="shared" si="3"/>
         <v>2.197951846606384E-4</v>
       </c>
-      <c r="C16" s="110">
+      <c r="C16" s="94">
         <f t="shared" si="0"/>
         <v>0.72532410938010672</v>
       </c>
-      <c r="D16" s="98">
+      <c r="D16" s="83">
         <f t="shared" si="1"/>
         <v>0.51288159630076657</v>
       </c>
-      <c r="E16" s="98">
+      <c r="E16" s="83">
         <f t="shared" si="4"/>
         <v>0.39892826015905875</v>
       </c>
@@ -4785,23 +4760,23 @@
         <v>0.28208487796542164</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="52">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="40">
         <v>33</v>
       </c>
-      <c r="B17" s="54">
+      <c r="B17" s="42">
         <f t="shared" si="3"/>
         <v>1.8701403163821613E-4</v>
       </c>
-      <c r="C17" s="110">
+      <c r="C17" s="94">
         <f t="shared" si="0"/>
         <v>0.61714630440611318</v>
       </c>
-      <c r="D17" s="98">
+      <c r="D17" s="83">
         <f t="shared" si="1"/>
         <v>0.4363883368297799</v>
       </c>
-      <c r="E17" s="98">
+      <c r="E17" s="83">
         <f t="shared" si="4"/>
         <v>0.33943046742336225</v>
       </c>
@@ -4810,23 +4785,23 @@
         <v>0.24001358525637895</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="52">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="40">
         <v>39</v>
       </c>
-      <c r="B18" s="54">
+      <c r="B18" s="42">
         <f t="shared" si="3"/>
         <v>1.6421698613531326E-4</v>
       </c>
-      <c r="C18" s="110">
+      <c r="C18" s="94">
         <f t="shared" si="0"/>
         <v>0.54191605424653377</v>
       </c>
-      <c r="D18" s="98">
+      <c r="D18" s="83">
         <f t="shared" si="1"/>
         <v>0.38319251679158095</v>
       </c>
-      <c r="E18" s="98">
+      <c r="E18" s="83">
         <f t="shared" si="4"/>
         <v>0.29805382983559359</v>
       </c>
@@ -4835,7 +4810,7 @@
         <v>0.21075588423536953</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>238</v>
       </c>
@@ -4860,26 +4835,26 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="37.109375" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" customWidth="1"/>
+    <col min="1" max="1" width="37.1640625" customWidth="1"/>
+    <col min="4" max="4" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="101" t="s">
+    <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="86" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="108" t="s">
+    <row r="2" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="93" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="21" x14ac:dyDescent="0.4">
-      <c r="A3" s="101"/>
-    </row>
-    <row r="4" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="A3" s="86"/>
+    </row>
+    <row r="4" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>197</v>
       </c>
@@ -4908,70 +4883,70 @@
         <v>228</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>200</v>
       </c>
-      <c r="B5" s="102">
+      <c r="B5" s="87">
         <v>5</v>
       </c>
-      <c r="C5" s="102">
-        <v>0</v>
-      </c>
-      <c r="D5" s="103">
+      <c r="C5" s="87">
+        <v>0</v>
+      </c>
+      <c r="D5" s="88">
         <v>10</v>
       </c>
-      <c r="E5" s="102" t="s">
+      <c r="E5" s="87" t="s">
         <v>201</v>
       </c>
-      <c r="F5" s="102" t="s">
+      <c r="F5" s="87" t="s">
         <v>202</v>
       </c>
-      <c r="G5" s="102" t="s">
+      <c r="G5" s="87" t="s">
         <v>203</v>
       </c>
-      <c r="H5" s="102" t="s">
+      <c r="H5" s="87" t="s">
         <v>204</v>
       </c>
-      <c r="I5" s="104" t="str">
+      <c r="I5" s="89" t="str">
         <f>DEC2HEX(O17,2)</f>
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>205</v>
       </c>
-      <c r="B6" s="105">
+      <c r="B6" s="90">
         <f>B5</f>
         <v>5</v>
       </c>
-      <c r="C6" s="105">
+      <c r="C6" s="90">
         <f>C5</f>
         <v>0</v>
       </c>
-      <c r="D6" s="105">
+      <c r="D6" s="90">
         <f>_xlfn.BITOR(HEX2DEC(D5), HEX2DEC(80))</f>
         <v>144</v>
       </c>
-      <c r="E6" s="105">
+      <c r="E6" s="90">
         <f>HEX2DEC(E5)</f>
         <v>0</v>
       </c>
-      <c r="F6" s="105">
+      <c r="F6" s="90">
         <f t="shared" ref="F6:H6" si="0">HEX2DEC(F5)</f>
         <v>1</v>
       </c>
-      <c r="G6" s="105">
+      <c r="G6" s="90">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="H6" s="105">
+      <c r="H6" s="90">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>206</v>
       </c>
@@ -4979,15 +4954,15 @@
         <v>207</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B9" s="106">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B9" s="91">
         <f>B6</f>
         <v>5</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
-      <c r="D9" s="106">
+      <c r="D9" s="91">
         <f>C6</f>
         <v>0</v>
       </c>
@@ -4995,7 +4970,7 @@
         <f>C17</f>
         <v>105</v>
       </c>
-      <c r="F9" s="106">
+      <c r="F9" s="91">
         <f>D6</f>
         <v>144</v>
       </c>
@@ -5003,7 +4978,7 @@
         <f>E17</f>
         <v>24</v>
       </c>
-      <c r="H9" s="107">
+      <c r="H9" s="92">
         <f>E6</f>
         <v>0</v>
       </c>
@@ -5011,7 +4986,7 @@
         <f>G17</f>
         <v>119</v>
       </c>
-      <c r="J9" s="107">
+      <c r="J9" s="92">
         <f>F6</f>
         <v>1</v>
       </c>
@@ -5019,7 +4994,7 @@
         <f>I17</f>
         <v>66</v>
       </c>
-      <c r="L9" s="107">
+      <c r="L9" s="92">
         <f>G6</f>
         <v>20</v>
       </c>
@@ -5027,7 +5002,7 @@
         <f>K17</f>
         <v>64</v>
       </c>
-      <c r="N9" s="107">
+      <c r="N9" s="92">
         <f>H6</f>
         <v>5</v>
       </c>
@@ -5036,7 +5011,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>208</v>
       </c>
@@ -5097,7 +5072,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>209</v>
       </c>
@@ -5158,7 +5133,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>210</v>
       </c>
@@ -5219,7 +5194,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>211</v>
       </c>
@@ -5280,7 +5255,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>212</v>
       </c>
@@ -5341,7 +5316,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>213</v>
       </c>
@@ -5402,7 +5377,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>214</v>
       </c>
@@ -5463,7 +5438,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>215</v>
       </c>
@@ -5524,7 +5499,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>216</v>
       </c>
@@ -5541,42 +5516,42 @@
         <v>228</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>218</v>
       </c>
-      <c r="B21" s="102" t="s">
+      <c r="B21" s="87" t="s">
         <v>204</v>
       </c>
-      <c r="C21" s="102" t="s">
+      <c r="C21" s="87" t="s">
         <v>219</v>
       </c>
-      <c r="D21" s="102" t="s">
+      <c r="D21" s="87" t="s">
         <v>220</v>
       </c>
-      <c r="E21" s="104" t="str">
+      <c r="E21" s="89" t="str">
         <f>DEC2HEX(G33,2)</f>
         <v>6F</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>221</v>
       </c>
-      <c r="B22" s="105" t="str">
+      <c r="B22" s="90" t="str">
         <f>B21</f>
         <v>05</v>
       </c>
-      <c r="C22" s="105" t="str">
+      <c r="C22" s="90" t="str">
         <f>C21</f>
         <v>0</v>
       </c>
-      <c r="D22" s="105">
+      <c r="D22" s="90">
         <f>HEX2DEC(D21)</f>
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>206</v>
       </c>
@@ -5584,15 +5559,15 @@
         <v>207</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B25" s="106" t="str">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B25" s="91" t="str">
         <f>B22</f>
         <v>05</v>
       </c>
       <c r="C25">
         <v>0</v>
       </c>
-      <c r="D25" s="106" t="str">
+      <c r="D25" s="91" t="str">
         <f>C22</f>
         <v>0</v>
       </c>
@@ -5600,7 +5575,7 @@
         <f>C33</f>
         <v>105</v>
       </c>
-      <c r="F25" s="106">
+      <c r="F25" s="91">
         <f>D22</f>
         <v>6</v>
       </c>
@@ -5608,12 +5583,12 @@
         <f>E33</f>
         <v>24</v>
       </c>
-      <c r="H25" s="25"/>
-      <c r="J25" s="25"/>
-      <c r="L25" s="25"/>
-      <c r="N25" s="25"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H25" s="23"/>
+      <c r="J25" s="23"/>
+      <c r="L25" s="23"/>
+      <c r="N25" s="23"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>208</v>
       </c>
@@ -5642,7 +5617,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>209</v>
       </c>
@@ -5671,7 +5646,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>210</v>
       </c>
@@ -5700,7 +5675,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>211</v>
       </c>
@@ -5729,7 +5704,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>212</v>
       </c>
@@ -5758,7 +5733,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>213</v>
       </c>
@@ -5787,7 +5762,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>214</v>
       </c>
@@ -5816,7 +5791,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>215</v>
       </c>
@@ -5859,14 +5834,14 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.88671875" customWidth="1"/>
+    <col min="1" max="1" width="12.83203125" customWidth="1"/>
     <col min="2" max="2" width="12.6640625" customWidth="1"/>
     <col min="3" max="3" width="123.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>24</v>
       </c>
@@ -5874,19 +5849,19 @@
         <v>190</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="11"/>
       <c r="B2" s="12"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C3" s="17" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C3" s="16" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B4" s="17"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B4" s="16"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>25</v>
       </c>
@@ -5897,8 +5872,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="18" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="14" t="s">
         <v>185</v>
       </c>
       <c r="B6" t="s">
@@ -5908,7 +5883,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>222</v>
       </c>
@@ -5919,8 +5894,8 @@
         <v>223</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="18" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="14" t="s">
         <v>236</v>
       </c>
       <c r="B8" t="s">
@@ -5930,7 +5905,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>240</v>
       </c>
@@ -5941,7 +5916,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>243</v>
       </c>

</xml_diff>